<commit_message>
do uzgodnienia - pytania do architekta
</commit_message>
<xml_diff>
--- a/plan/Mati - do uzgodnienia.xlsx
+++ b/plan/Mati - do uzgodnienia.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="60" windowWidth="11295" windowHeight="5580" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="2505" windowWidth="13095" windowHeight="4200"/>
   </bookViews>
   <sheets>
     <sheet name="Do uzgodnienia" sheetId="1" r:id="rId1"/>
@@ -12,11 +12,12 @@
     <sheet name="Do ustalenia" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
+  <oleSize ref="A13:G21"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="80">
   <si>
     <t>Pralnia i suszarnia</t>
   </si>
@@ -90,9 +91,6 @@
     <t>Kanalizacja</t>
   </si>
   <si>
-    <t>sąsiedzi</t>
-  </si>
-  <si>
     <t>Prąd</t>
   </si>
   <si>
@@ -123,9 +121,6 @@
     <t>Przekształcenie działki</t>
   </si>
   <si>
-    <t>MKU</t>
-  </si>
-  <si>
     <t>dla dwóch osób nie ma potrzeby</t>
   </si>
   <si>
@@ -150,9 +145,6 @@
     <t>Dodatkowa warstwa pustaków do podwyższenia pomieszczeń na poddaszu?</t>
   </si>
   <si>
-    <t>tak</t>
-  </si>
-  <si>
     <t>architekt</t>
   </si>
   <si>
@@ -213,13 +205,58 @@
     <t>pozwala na niskie zużycie energii potrzebnej do ogrzewania</t>
   </si>
   <si>
-    <t>Wewnętzne instalacje</t>
-  </si>
-  <si>
     <t>Jakie decyzje potrzebne do projektu (rodzaj ogrzewania, czy kominek podłączony do ogrzewania, wentylacja mechaniczna)?</t>
   </si>
   <si>
     <t>Zmiany konstrukcyjne</t>
+  </si>
+  <si>
+    <t>Wewnętrzne instalacje</t>
+  </si>
+  <si>
+    <t>Działka</t>
+  </si>
+  <si>
+    <t>Drenaż</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Czy jest potrzebny projekt drenażu? Jak zmienia się projekt drenażu w przypadku robienia piwnicy? </t>
+  </si>
+  <si>
+    <t>Podkategoria</t>
+  </si>
+  <si>
+    <t>Źródło informacji</t>
+  </si>
+  <si>
+    <t>Termin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wynik </t>
+  </si>
+  <si>
+    <t>można w dowolnej chwili dokupić kosztorys i inne dodatki</t>
+  </si>
+  <si>
+    <t>Przekształcenie działki na budowlaną</t>
+  </si>
+  <si>
+    <t>Czy architekt się tym zajmie? Ile to może potrwać?</t>
+  </si>
+  <si>
+    <t>TAK</t>
+  </si>
+  <si>
+    <t>to dobry pomysł</t>
+  </si>
+  <si>
+    <t>Łazienka</t>
+  </si>
+  <si>
+    <t>Drzwi oddzielające ubikację</t>
+  </si>
+  <si>
+    <t>Odpowiednie rozplanowanie przestrzeni w łazience</t>
   </si>
 </sst>
 </file>
@@ -245,15 +282,27 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF4CFE22"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -261,28 +310,62 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF4CFE22"/>
+    </mruColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -571,283 +654,388 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P23"/>
+  <dimension ref="A1:P24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="17" customWidth="1"/>
-    <col min="2" max="2" width="48" customWidth="1"/>
-    <col min="3" max="3" width="27.85546875" customWidth="1"/>
-    <col min="4" max="4" width="18" customWidth="1"/>
-    <col min="5" max="5" width="8" customWidth="1"/>
+    <col min="1" max="1" width="13" customWidth="1"/>
+    <col min="2" max="2" width="33.140625" customWidth="1"/>
+    <col min="3" max="3" width="19.28515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" customWidth="1"/>
+    <col min="5" max="5" width="7.7109375" customWidth="1"/>
     <col min="6" max="6" width="18.28515625" customWidth="1"/>
     <col min="7" max="7" width="8" customWidth="1"/>
     <col min="8" max="8" width="19.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:16" s="8" customFormat="1">
+      <c r="A1" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="7" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="30">
-      <c r="A2" t="s">
+    <row r="2" spans="1:16" ht="60">
+      <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="5"/>
+      <c r="P2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" ht="60">
+      <c r="A3" s="4"/>
+      <c r="B3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="P3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" ht="105">
+      <c r="A4" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+      <c r="P4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" ht="30">
+      <c r="A5" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="3"/>
-      <c r="P2" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" ht="30">
-      <c r="B3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="P3" t="s">
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="P5" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="60">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" s="2" t="s">
+    <row r="6" spans="1:16">
+      <c r="A6" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="P4" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" ht="30">
-      <c r="A5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" s="2" t="s">
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+      <c r="P6" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" ht="75">
+      <c r="A7" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="P5" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16">
-      <c r="A6" t="s">
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+    </row>
+    <row r="8" spans="1:16" ht="30">
+      <c r="A8" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B6" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" s="2" t="s">
+      <c r="B8" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+    </row>
+    <row r="9" spans="1:16" ht="105">
+      <c r="A9" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="H9" s="6"/>
+    </row>
+    <row r="10" spans="1:16">
+      <c r="A10" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+    </row>
+    <row r="11" spans="1:16" s="11" customFormat="1">
+      <c r="A11" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="P6" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" ht="45">
-      <c r="A7" t="s">
-        <v>16</v>
-      </c>
-      <c r="B7" t="s">
-        <v>18</v>
-      </c>
-      <c r="D7" s="2" t="s">
+      <c r="B11" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-    </row>
-    <row r="8" spans="1:16">
-      <c r="A8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B8" t="s">
-        <v>19</v>
-      </c>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-    </row>
-    <row r="9" spans="1:16" ht="75">
-      <c r="A9" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9" t="s">
-        <v>20</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="H9" s="2"/>
-    </row>
-    <row r="10" spans="1:16">
-      <c r="A10" t="s">
-        <v>16</v>
-      </c>
-      <c r="B10" t="s">
-        <v>21</v>
-      </c>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-    </row>
-    <row r="11" spans="1:16">
-      <c r="A11" t="s">
-        <v>42</v>
-      </c>
-      <c r="B11" t="s">
-        <v>43</v>
-      </c>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16">
-      <c r="A12" t="s">
-        <v>55</v>
-      </c>
-      <c r="B12" t="s">
-        <v>56</v>
-      </c>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-      <c r="H12" t="s">
+      <c r="C11" s="10"/>
+      <c r="D11" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="E11" s="10"/>
+      <c r="F11" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="G11" s="10"/>
+      <c r="H11" s="10" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" s="11" customFormat="1">
+      <c r="A12" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="C12" s="10"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="10"/>
+      <c r="H12" s="9" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" ht="60">
+      <c r="A13" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="E13" s="6" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="13" spans="1:16">
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
     </row>
     <row r="14" spans="1:16">
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
+      <c r="A14" s="4"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
     </row>
     <row r="15" spans="1:16">
-      <c r="E15" s="2"/>
-      <c r="G15" s="2"/>
+      <c r="A15" s="4"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="4"/>
     </row>
     <row r="16" spans="1:16">
-      <c r="E16" s="2"/>
-      <c r="G16" s="2"/>
-    </row>
-    <row r="17" spans="5:7">
-      <c r="E17" s="2"/>
-      <c r="G17" s="2"/>
-    </row>
-    <row r="18" spans="5:7">
-      <c r="E18" s="2"/>
-      <c r="G18" s="2"/>
-    </row>
-    <row r="19" spans="5:7">
-      <c r="E19" s="2"/>
-      <c r="G19" s="2"/>
-    </row>
-    <row r="20" spans="5:7">
-      <c r="E20" s="2"/>
-      <c r="G20" s="2"/>
-    </row>
-    <row r="21" spans="5:7">
-      <c r="E21" s="2"/>
-      <c r="G21" s="2"/>
-    </row>
-    <row r="22" spans="5:7">
-      <c r="E22" s="2"/>
-      <c r="G22" s="2"/>
-    </row>
-    <row r="23" spans="5:7">
-      <c r="E23" s="2"/>
+      <c r="A16" s="4"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="4"/>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" s="4"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="4"/>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" s="4"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="4"/>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19" s="4"/>
+      <c r="B19" s="4"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="4"/>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20" s="4"/>
+      <c r="B20" s="4"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="4"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="4"/>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="A21" s="4"/>
+      <c r="B21" s="4"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="4"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="4"/>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="A22" s="4"/>
+      <c r="B22" s="4"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="4"/>
+      <c r="G22" s="6"/>
+      <c r="H22" s="4"/>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="A23" s="4"/>
+      <c r="B23" s="4"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="4"/>
+      <c r="G23" s="4"/>
+      <c r="H23" s="4"/>
+    </row>
+    <row r="24" spans="1:8">
+      <c r="A24" s="4"/>
+      <c r="B24" s="4"/>
+      <c r="C24" s="6"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="4"/>
+      <c r="F24" s="4"/>
+      <c r="G24" s="4"/>
+      <c r="H24" s="4"/>
     </row>
   </sheetData>
   <dataValidations count="1">
@@ -862,109 +1050,231 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:G7"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:G4"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="19.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.42578125" customWidth="1"/>
+    <col min="3" max="3" width="38.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.42578125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7">
-      <c r="A2" t="s">
+    <row r="1" spans="1:5">
+      <c r="A1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2" s="6"/>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="4"/>
+      <c r="B3" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="G2" t="s">
+      <c r="C3" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E3" s="6"/>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="4"/>
+      <c r="B4" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E4" s="6"/>
+    </row>
+    <row r="5" spans="1:5" ht="60">
+      <c r="A5" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" s="4" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="B3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C3" t="s">
-        <v>24</v>
-      </c>
-      <c r="G3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="B4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C4" t="s">
-        <v>24</v>
-      </c>
-      <c r="G4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="A5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B5" t="s">
+      <c r="E5" s="6" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E6" s="6"/>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C5" t="s">
-        <v>28</v>
-      </c>
-      <c r="G5" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="A6" t="s">
-        <v>29</v>
-      </c>
-      <c r="C6" t="s">
+      <c r="B7" s="4"/>
+      <c r="C7" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D7" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="G6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="A7" t="s">
-        <v>34</v>
-      </c>
-      <c r="C7" t="s">
-        <v>35</v>
-      </c>
-      <c r="G7" t="s">
-        <v>32</v>
-      </c>
+      <c r="E7" s="6"/>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="4"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="6"/>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="4"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="6"/>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="4"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="6"/>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="4"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="6"/>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="4"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="6"/>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="4"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="6"/>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="4"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="6"/>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="4"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="6"/>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="4"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="6"/>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="4"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="6"/>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="4"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="6"/>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" s="4"/>
+      <c r="B19" s="4"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="6"/>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="4"/>
+      <c r="B20" s="4"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="32.85546875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="34.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.85546875" style="1" customWidth="1"/>
     <col min="4" max="4" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -973,85 +1283,104 @@
         <v>22</v>
       </c>
       <c r="B1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>51</v>
-      </c>
       <c r="E1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="G1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="60">
       <c r="B2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>52</v>
+        <v>24</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>49</v>
       </c>
       <c r="E2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="G2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="45">
       <c r="B3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>45</v>
+        <v>25</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="G3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="45">
       <c r="B4" t="s">
-        <v>47</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="G4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="45">
       <c r="A5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>46</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="45">
       <c r="A6" t="s">
-        <v>67</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>54</v>
+        <v>63</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="75">
       <c r="A7" t="s">
+        <v>64</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="60">
+      <c r="A8" t="s">
         <v>65</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="B8" t="s">
         <v>66</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="30">
+      <c r="B9" t="s">
+        <v>73</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>74</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Lista do uzgodnienia - podział na kategorie Adaptacja i Wykończenie
</commit_message>
<xml_diff>
--- a/plan/Mati - do uzgodnienia.xlsx
+++ b/plan/Mati - do uzgodnienia.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2505" windowWidth="13095" windowHeight="4200"/>
+    <workbookView visibility="veryHidden" xWindow="0" yWindow="0" windowWidth="13095" windowHeight="6390"/>
   </bookViews>
   <sheets>
     <sheet name="Do uzgodnienia" sheetId="1" r:id="rId1"/>
@@ -12,12 +12,12 @@
     <sheet name="Do ustalenia" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <oleSize ref="A13:G21"/>
+  <oleSize ref="A1:G3"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="82">
   <si>
     <t>Pralnia i suszarnia</t>
   </si>
@@ -257,6 +257,12 @@
   </si>
   <si>
     <t>Odpowiednie rozplanowanie przestrzeni w łazience</t>
+  </si>
+  <si>
+    <t>Okna</t>
+  </si>
+  <si>
+    <t>Drewniane czy plastikowe (lub plastikowe stylizowane)?</t>
   </si>
 </sst>
 </file>
@@ -656,8 +662,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:P24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -927,10 +933,14 @@
       <c r="G13" s="6"/>
       <c r="H13" s="6"/>
     </row>
-    <row r="14" spans="1:16">
-      <c r="A14" s="4"/>
+    <row r="14" spans="1:16" ht="60">
+      <c r="A14" s="4" t="s">
+        <v>80</v>
+      </c>
       <c r="B14" s="4"/>
-      <c r="C14" s="6"/>
+      <c r="C14" s="6" t="s">
+        <v>81</v>
+      </c>
       <c r="D14" s="6"/>
       <c r="E14" s="6"/>
       <c r="F14" s="6"/>
@@ -1345,7 +1355,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="45">
+    <row r="6" spans="1:7">
       <c r="A6" t="s">
         <v>63</v>
       </c>

</xml_diff>

<commit_message>
jeszcze raz update 'Do uzgodnienia' z podziałem na etapy
</commit_message>
<xml_diff>
--- a/plan/Mati - do uzgodnienia.xlsx
+++ b/plan/Mati - do uzgodnienia.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView visibility="veryHidden" xWindow="0" yWindow="0" windowWidth="13095" windowHeight="6390"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13095" windowHeight="6390"/>
   </bookViews>
   <sheets>
     <sheet name="Do uzgodnienia" sheetId="1" r:id="rId1"/>
@@ -12,12 +12,11 @@
     <sheet name="Do ustalenia" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <oleSize ref="A1:G3"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="89">
   <si>
     <t>Pralnia i suszarnia</t>
   </si>
@@ -70,9 +69,6 @@
     <t>Ogrzewanie</t>
   </si>
   <si>
-    <t>Jakie paliwo?</t>
-  </si>
-  <si>
     <t>Jaka instalacja? (podłogowe?)</t>
   </si>
   <si>
@@ -263,13 +259,37 @@
   </si>
   <si>
     <t>Drewniane czy plastikowe (lub plastikowe stylizowane)?</t>
+  </si>
+  <si>
+    <t>Etap</t>
+  </si>
+  <si>
+    <t>Adaptacja</t>
+  </si>
+  <si>
+    <t>Wykończenie</t>
+  </si>
+  <si>
+    <t>Zamiast garderoby na poddaszu</t>
+  </si>
+  <si>
+    <t>W razie Niemca</t>
+  </si>
+  <si>
+    <t>Umiejscowienie toalety</t>
+  </si>
+  <si>
+    <t>Pod skosem po podwyższeniu ścianki kolankowej</t>
+  </si>
+  <si>
+    <t>Jakie paliwo? Gaz, węgiel, drewno, pompa ciepła, panele, kombinacje powyższych, inne</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -286,6 +306,13 @@
       <family val="2"/>
       <charset val="238"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+      <charset val="238"/>
     </font>
   </fonts>
   <fills count="4">
@@ -308,7 +335,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -331,11 +358,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -349,17 +389,32 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -660,397 +715,677 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P24"/>
+  <dimension ref="A1:S45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="13" customWidth="1"/>
-    <col min="2" max="2" width="33.140625" customWidth="1"/>
-    <col min="3" max="3" width="19.28515625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="11.42578125" customWidth="1"/>
-    <col min="5" max="5" width="7.7109375" customWidth="1"/>
-    <col min="6" max="6" width="18.28515625" customWidth="1"/>
-    <col min="7" max="7" width="8" customWidth="1"/>
-    <col min="8" max="8" width="19.5703125" customWidth="1"/>
+    <col min="1" max="1" width="14" style="16" customWidth="1"/>
+    <col min="2" max="2" width="16" style="20" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.7109375" style="21" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.7109375" style="21" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17" style="20" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.7109375" style="20" customWidth="1"/>
+    <col min="7" max="7" width="18.28515625" style="20" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" style="20" customWidth="1"/>
+    <col min="9" max="9" width="19.5703125" style="20" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="8" customFormat="1">
+    <row r="1" spans="1:19" s="11" customFormat="1">
       <c r="A1" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="B1" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="C1" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="D1" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="E1" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="F1" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="G1" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="H1" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="I1" s="10" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="60">
-      <c r="A2" s="4" t="s">
+    <row r="2" spans="1:19" ht="51">
+      <c r="A2" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="B2" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="C2" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="D2" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="E2" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="F2" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
+      <c r="I2" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="Q2" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="S2" s="15" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" ht="51">
+      <c r="A3" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="B3" s="17"/>
+      <c r="C3" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="F3" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="G3" s="18"/>
+      <c r="H3" s="18"/>
+      <c r="I3" s="18"/>
+      <c r="Q3" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="S3" s="15" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" ht="51">
+      <c r="A4" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="18"/>
+      <c r="E4" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="F4" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="G4" s="18" t="s">
+        <v>85</v>
+      </c>
+      <c r="H4" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="5"/>
-      <c r="P2" t="s">
+      <c r="I4" s="18"/>
+      <c r="Q4" s="15" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" ht="25.5">
+      <c r="A5" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="B5" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="18"/>
+      <c r="E5" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="F5" s="18"/>
+      <c r="G5" s="18"/>
+      <c r="H5" s="18"/>
+      <c r="I5" s="18"/>
+      <c r="Q5" s="15" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" ht="38.25">
+      <c r="A6" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="B6" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="D6" s="18"/>
+      <c r="E6" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="F6" s="18"/>
+      <c r="G6" s="18"/>
+      <c r="H6" s="18"/>
+      <c r="I6" s="18"/>
+      <c r="Q6" s="15" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" ht="38.25">
+      <c r="A7" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="B7" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="18"/>
+      <c r="E7" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="F7" s="18"/>
+      <c r="G7" s="18"/>
+      <c r="H7" s="18"/>
+      <c r="I7" s="18"/>
+    </row>
+    <row r="8" spans="1:19" ht="25.5">
+      <c r="A8" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="B8" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" s="18"/>
+      <c r="E8" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="F8" s="18" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="3" spans="1:16" ht="60">
-      <c r="A3" s="4"/>
-      <c r="B3" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-      <c r="P3" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" ht="105">
-      <c r="A4" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="6"/>
-      <c r="P4" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" ht="30">
-      <c r="A5" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6"/>
-      <c r="H5" s="6"/>
-      <c r="P5" t="s">
+      <c r="G8" s="18"/>
+      <c r="H8" s="18"/>
+      <c r="I8" s="18"/>
+    </row>
+    <row r="9" spans="1:19" ht="51">
+      <c r="A9" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="B9" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" s="18"/>
+      <c r="E9" s="18" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="6" spans="1:16">
-      <c r="A6" s="4" t="s">
+      <c r="F9" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="G9" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="H9" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="I9" s="18"/>
+    </row>
+    <row r="10" spans="1:19">
+      <c r="A10" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="B10" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="6"/>
-      <c r="P6" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" ht="75">
-      <c r="A7" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6" t="s">
+      <c r="C10" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="18"/>
+      <c r="H10" s="18"/>
+      <c r="I10" s="18"/>
+    </row>
+    <row r="11" spans="1:19" s="19" customFormat="1" ht="38.25">
+      <c r="A11" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="B11" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
-    </row>
-    <row r="8" spans="1:16" ht="30">
-      <c r="A8" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6" t="s">
+      <c r="C11" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="D11" s="14"/>
+      <c r="E11" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="F11" s="14"/>
+      <c r="G11" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="H11" s="14"/>
+      <c r="I11" s="14" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" s="19" customFormat="1" ht="38.25">
+      <c r="A12" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="D12" s="14"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="14"/>
+      <c r="I12" s="14" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" ht="51">
+      <c r="A13" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="B13" s="17" t="s">
         <v>76</v>
       </c>
-      <c r="E8" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
-    </row>
-    <row r="9" spans="1:16" ht="105">
-      <c r="A9" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="F9" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="G9" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="H9" s="6"/>
-    </row>
-    <row r="10" spans="1:16">
-      <c r="A10" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
-    </row>
-    <row r="11" spans="1:16" s="11" customFormat="1">
-      <c r="A11" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="B11" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="C11" s="10"/>
-      <c r="D11" s="10" t="s">
-        <v>75</v>
-      </c>
-      <c r="E11" s="10"/>
-      <c r="F11" s="10" t="s">
-        <v>75</v>
-      </c>
-      <c r="G11" s="10"/>
-      <c r="H11" s="10" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" s="11" customFormat="1">
-      <c r="A12" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="B12" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="C12" s="10"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="10"/>
-      <c r="F12" s="10"/>
-      <c r="G12" s="10"/>
-      <c r="H12" s="9" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" ht="60">
-      <c r="A13" s="4" t="s">
+      <c r="C13" s="18" t="s">
         <v>77</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="D13" s="18" t="s">
         <v>78</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="E13" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="F13" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="G13" s="18"/>
+      <c r="H13" s="18"/>
+      <c r="I13" s="18"/>
+    </row>
+    <row r="14" spans="1:19" ht="51">
+      <c r="A14" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="B14" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="C14" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="D14" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="E14" s="14"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="14"/>
+      <c r="H14" s="14"/>
+      <c r="I14" s="14" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" ht="51">
+      <c r="A15" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="B15" s="17" t="s">
         <v>79</v>
       </c>
-      <c r="D13" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="E13" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="F13" s="6"/>
-      <c r="G13" s="6"/>
-      <c r="H13" s="6"/>
-    </row>
-    <row r="14" spans="1:16" ht="60">
-      <c r="A14" s="4" t="s">
+      <c r="C15" s="18"/>
+      <c r="D15" s="18" t="s">
         <v>80</v>
       </c>
-      <c r="B14" s="4"/>
-      <c r="C14" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="6"/>
-      <c r="H14" s="6"/>
-    </row>
-    <row r="15" spans="1:16">
-      <c r="A15" s="4"/>
-      <c r="B15" s="4"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="6"/>
-      <c r="H15" s="4"/>
-    </row>
-    <row r="16" spans="1:16">
-      <c r="A16" s="4"/>
-      <c r="B16" s="4"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="4"/>
-      <c r="G16" s="6"/>
-      <c r="H16" s="4"/>
-    </row>
-    <row r="17" spans="1:8">
-      <c r="A17" s="4"/>
-      <c r="B17" s="4"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="6"/>
-      <c r="F17" s="4"/>
-      <c r="G17" s="6"/>
-      <c r="H17" s="4"/>
-    </row>
-    <row r="18" spans="1:8">
-      <c r="A18" s="4"/>
-      <c r="B18" s="4"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="4"/>
-      <c r="G18" s="6"/>
-      <c r="H18" s="4"/>
-    </row>
-    <row r="19" spans="1:8">
-      <c r="A19" s="4"/>
-      <c r="B19" s="4"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="6"/>
-      <c r="F19" s="4"/>
-      <c r="G19" s="6"/>
-      <c r="H19" s="4"/>
-    </row>
-    <row r="20" spans="1:8">
-      <c r="A20" s="4"/>
-      <c r="B20" s="4"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="4"/>
-      <c r="E20" s="6"/>
-      <c r="F20" s="4"/>
-      <c r="G20" s="6"/>
-      <c r="H20" s="4"/>
-    </row>
-    <row r="21" spans="1:8">
-      <c r="A21" s="4"/>
-      <c r="B21" s="4"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="4"/>
-      <c r="E21" s="6"/>
-      <c r="F21" s="4"/>
-      <c r="G21" s="6"/>
-      <c r="H21" s="4"/>
-    </row>
-    <row r="22" spans="1:8">
-      <c r="A22" s="4"/>
-      <c r="B22" s="4"/>
-      <c r="C22" s="6"/>
-      <c r="D22" s="4"/>
-      <c r="E22" s="6"/>
-      <c r="F22" s="4"/>
-      <c r="G22" s="6"/>
-      <c r="H22" s="4"/>
-    </row>
-    <row r="23" spans="1:8">
-      <c r="A23" s="4"/>
-      <c r="B23" s="4"/>
-      <c r="C23" s="6"/>
-      <c r="D23" s="4"/>
-      <c r="E23" s="6"/>
-      <c r="F23" s="4"/>
-      <c r="G23" s="4"/>
-      <c r="H23" s="4"/>
-    </row>
-    <row r="24" spans="1:8">
-      <c r="A24" s="4"/>
-      <c r="B24" s="4"/>
-      <c r="C24" s="6"/>
-      <c r="D24" s="4"/>
-      <c r="E24" s="4"/>
-      <c r="F24" s="4"/>
-      <c r="G24" s="4"/>
-      <c r="H24" s="4"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="18"/>
+      <c r="G15" s="18"/>
+      <c r="H15" s="18"/>
+      <c r="I15" s="18"/>
+    </row>
+    <row r="16" spans="1:19">
+      <c r="B16" s="17"/>
+      <c r="C16" s="18"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="16"/>
+      <c r="F16" s="18"/>
+      <c r="G16" s="16"/>
+      <c r="H16" s="18"/>
+      <c r="I16" s="16"/>
+    </row>
+    <row r="17" spans="2:9">
+      <c r="B17" s="17"/>
+      <c r="C17" s="18"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="16"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="16"/>
+      <c r="H17" s="18"/>
+      <c r="I17" s="16"/>
+    </row>
+    <row r="18" spans="2:9">
+      <c r="B18" s="17"/>
+      <c r="C18" s="18"/>
+      <c r="D18" s="18"/>
+      <c r="E18" s="16"/>
+      <c r="F18" s="18"/>
+      <c r="G18" s="16"/>
+      <c r="H18" s="18"/>
+      <c r="I18" s="16"/>
+    </row>
+    <row r="19" spans="2:9">
+      <c r="B19" s="17"/>
+      <c r="C19" s="18"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="16"/>
+      <c r="F19" s="18"/>
+      <c r="G19" s="16"/>
+      <c r="H19" s="18"/>
+      <c r="I19" s="16"/>
+    </row>
+    <row r="20" spans="2:9">
+      <c r="B20" s="17"/>
+      <c r="C20" s="18"/>
+      <c r="D20" s="18"/>
+      <c r="E20" s="16"/>
+      <c r="F20" s="18"/>
+      <c r="G20" s="16"/>
+      <c r="H20" s="18"/>
+      <c r="I20" s="16"/>
+    </row>
+    <row r="21" spans="2:9">
+      <c r="B21" s="17"/>
+      <c r="C21" s="18"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="16"/>
+      <c r="F21" s="18"/>
+      <c r="G21" s="16"/>
+      <c r="H21" s="18"/>
+      <c r="I21" s="16"/>
+    </row>
+    <row r="22" spans="2:9">
+      <c r="B22" s="17"/>
+      <c r="C22" s="18"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="16"/>
+      <c r="F22" s="18"/>
+      <c r="G22" s="16"/>
+      <c r="H22" s="18"/>
+      <c r="I22" s="16"/>
+    </row>
+    <row r="23" spans="2:9">
+      <c r="B23" s="17"/>
+      <c r="C23" s="18"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="16"/>
+      <c r="F23" s="18"/>
+      <c r="G23" s="16"/>
+      <c r="H23" s="18"/>
+      <c r="I23" s="16"/>
+    </row>
+    <row r="24" spans="2:9">
+      <c r="B24" s="17"/>
+      <c r="C24" s="18"/>
+      <c r="D24" s="18"/>
+      <c r="E24" s="16"/>
+      <c r="F24" s="18"/>
+      <c r="G24" s="16"/>
+      <c r="H24" s="16"/>
+      <c r="I24" s="16"/>
+    </row>
+    <row r="25" spans="2:9">
+      <c r="B25" s="17"/>
+      <c r="C25" s="18"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="16"/>
+      <c r="F25" s="16"/>
+      <c r="G25" s="16"/>
+      <c r="H25" s="16"/>
+      <c r="I25" s="16"/>
+    </row>
+    <row r="26" spans="2:9">
+      <c r="B26" s="16"/>
+      <c r="C26" s="18"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="16"/>
+      <c r="F26" s="16"/>
+      <c r="G26" s="16"/>
+      <c r="H26" s="16"/>
+      <c r="I26" s="16"/>
+    </row>
+    <row r="27" spans="2:9">
+      <c r="B27" s="16"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="16"/>
+      <c r="F27" s="16"/>
+      <c r="G27" s="16"/>
+      <c r="H27" s="16"/>
+      <c r="I27" s="16"/>
+    </row>
+    <row r="28" spans="2:9">
+      <c r="B28" s="16"/>
+      <c r="C28" s="18"/>
+      <c r="D28" s="18"/>
+      <c r="E28" s="16"/>
+      <c r="F28" s="16"/>
+      <c r="G28" s="16"/>
+      <c r="H28" s="16"/>
+      <c r="I28" s="16"/>
+    </row>
+    <row r="29" spans="2:9">
+      <c r="B29" s="16"/>
+      <c r="C29" s="18"/>
+      <c r="D29" s="18"/>
+      <c r="E29" s="16"/>
+      <c r="F29" s="16"/>
+      <c r="G29" s="16"/>
+      <c r="H29" s="16"/>
+      <c r="I29" s="16"/>
+    </row>
+    <row r="30" spans="2:9">
+      <c r="B30" s="16"/>
+      <c r="C30" s="18"/>
+      <c r="D30" s="18"/>
+      <c r="E30" s="16"/>
+      <c r="F30" s="16"/>
+      <c r="G30" s="16"/>
+      <c r="H30" s="16"/>
+      <c r="I30" s="16"/>
+    </row>
+    <row r="31" spans="2:9">
+      <c r="B31" s="16"/>
+      <c r="C31" s="18"/>
+      <c r="D31" s="18"/>
+      <c r="E31" s="16"/>
+      <c r="F31" s="16"/>
+      <c r="G31" s="16"/>
+      <c r="H31" s="16"/>
+      <c r="I31" s="16"/>
+    </row>
+    <row r="32" spans="2:9">
+      <c r="B32" s="16"/>
+      <c r="C32" s="18"/>
+      <c r="D32" s="18"/>
+      <c r="E32" s="16"/>
+      <c r="F32" s="16"/>
+      <c r="G32" s="16"/>
+      <c r="H32" s="16"/>
+      <c r="I32" s="16"/>
+    </row>
+    <row r="33" spans="2:9">
+      <c r="B33" s="16"/>
+      <c r="C33" s="18"/>
+      <c r="D33" s="18"/>
+      <c r="E33" s="16"/>
+      <c r="F33" s="16"/>
+      <c r="G33" s="16"/>
+      <c r="H33" s="16"/>
+      <c r="I33" s="16"/>
+    </row>
+    <row r="34" spans="2:9">
+      <c r="B34" s="16"/>
+      <c r="C34" s="18"/>
+      <c r="D34" s="18"/>
+      <c r="E34" s="16"/>
+      <c r="F34" s="16"/>
+      <c r="G34" s="16"/>
+      <c r="H34" s="16"/>
+      <c r="I34" s="16"/>
+    </row>
+    <row r="35" spans="2:9">
+      <c r="B35" s="16"/>
+      <c r="C35" s="18"/>
+      <c r="D35" s="18"/>
+      <c r="E35" s="16"/>
+      <c r="F35" s="16"/>
+      <c r="G35" s="16"/>
+      <c r="H35" s="16"/>
+      <c r="I35" s="16"/>
+    </row>
+    <row r="36" spans="2:9">
+      <c r="B36" s="16"/>
+      <c r="C36" s="18"/>
+      <c r="D36" s="18"/>
+      <c r="E36" s="16"/>
+      <c r="F36" s="16"/>
+      <c r="G36" s="16"/>
+      <c r="H36" s="16"/>
+      <c r="I36" s="16"/>
+    </row>
+    <row r="37" spans="2:9">
+      <c r="B37" s="16"/>
+      <c r="C37" s="18"/>
+      <c r="D37" s="18"/>
+      <c r="E37" s="16"/>
+      <c r="F37" s="16"/>
+      <c r="G37" s="16"/>
+      <c r="H37" s="16"/>
+      <c r="I37" s="16"/>
+    </row>
+    <row r="38" spans="2:9">
+      <c r="B38" s="16"/>
+      <c r="C38" s="18"/>
+      <c r="D38" s="18"/>
+      <c r="E38" s="16"/>
+      <c r="F38" s="16"/>
+      <c r="G38" s="16"/>
+      <c r="H38" s="16"/>
+      <c r="I38" s="16"/>
+    </row>
+    <row r="39" spans="2:9">
+      <c r="B39" s="16"/>
+      <c r="C39" s="18"/>
+      <c r="D39" s="18"/>
+      <c r="E39" s="16"/>
+      <c r="F39" s="16"/>
+      <c r="G39" s="16"/>
+      <c r="H39" s="16"/>
+      <c r="I39" s="16"/>
+    </row>
+    <row r="40" spans="2:9">
+      <c r="B40" s="16"/>
+      <c r="C40" s="18"/>
+      <c r="D40" s="18"/>
+      <c r="E40" s="16"/>
+      <c r="F40" s="16"/>
+      <c r="G40" s="16"/>
+      <c r="H40" s="16"/>
+      <c r="I40" s="16"/>
+    </row>
+    <row r="41" spans="2:9">
+      <c r="B41" s="16"/>
+      <c r="C41" s="18"/>
+      <c r="D41" s="18"/>
+      <c r="E41" s="16"/>
+      <c r="F41" s="16"/>
+      <c r="G41" s="16"/>
+      <c r="H41" s="16"/>
+      <c r="I41" s="16"/>
+    </row>
+    <row r="42" spans="2:9">
+      <c r="B42" s="16"/>
+      <c r="C42" s="18"/>
+      <c r="D42" s="18"/>
+      <c r="E42" s="16"/>
+      <c r="F42" s="16"/>
+      <c r="G42" s="16"/>
+      <c r="H42" s="16"/>
+      <c r="I42" s="16"/>
+    </row>
+    <row r="43" spans="2:9">
+      <c r="B43" s="16"/>
+      <c r="C43" s="18"/>
+      <c r="D43" s="18"/>
+      <c r="E43" s="16"/>
+      <c r="F43" s="16"/>
+      <c r="G43" s="16"/>
+      <c r="H43" s="16"/>
+      <c r="I43" s="16"/>
+    </row>
+    <row r="44" spans="2:9">
+      <c r="B44" s="16"/>
+      <c r="C44" s="18"/>
+      <c r="D44" s="18"/>
+      <c r="E44" s="16"/>
+      <c r="F44" s="16"/>
+      <c r="G44" s="16"/>
+      <c r="H44" s="16"/>
+      <c r="I44" s="16"/>
+    </row>
+    <row r="45" spans="2:9">
+      <c r="B45" s="16"/>
+      <c r="C45" s="18"/>
+      <c r="D45" s="18"/>
+      <c r="E45" s="16"/>
+      <c r="F45" s="16"/>
+      <c r="G45" s="16"/>
+      <c r="H45" s="16"/>
+      <c r="I45" s="16"/>
     </row>
   </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E23 G2:G22">
-      <formula1>$P$2:$P$6</formula1>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F24 H2:H23">
+      <formula1>$Q$2:$Q$6</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A25">
+      <formula1>$S$2:$S$3</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1079,99 +1414,99 @@
         <v>9</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="5" t="s">
         <v>70</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>23</v>
-      </c>
       <c r="C2" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E2" s="6"/>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="4"/>
       <c r="B3" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E3" s="6"/>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="4"/>
       <c r="B4" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E4" s="6"/>
     </row>
     <row r="5" spans="1:5" ht="60">
       <c r="A5" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B5" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>27</v>
-      </c>
       <c r="D5" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B6" s="4"/>
       <c r="C6" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" s="4" t="s">
         <v>29</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>30</v>
       </c>
       <c r="E6" s="6"/>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B7" s="4"/>
       <c r="C7" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E7" s="6"/>
     </row>
@@ -1290,107 +1625,107 @@
   <sheetData>
     <row r="1" spans="1:7" ht="60">
       <c r="A1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="60">
       <c r="B2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="45">
       <c r="B3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="45">
       <c r="B4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="45">
       <c r="A5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="75">
       <c r="A7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="60">
       <c r="A8" t="s">
+        <v>64</v>
+      </c>
+      <c r="B8" t="s">
         <v>65</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" s="1" t="s">
         <v>66</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="30">
       <c r="B9" t="s">
+        <v>72</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>73</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>74</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
wybór ogrzewania - notatki
</commit_message>
<xml_diff>
--- a/plan/Mati - do uzgodnienia.xlsx
+++ b/plan/Mati - do uzgodnienia.xlsx
@@ -1,22 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13095" windowHeight="6390"/>
+    <workbookView xWindow="0" yWindow="2505" windowWidth="14145" windowHeight="4365" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Do uzgodnienia" sheetId="1" r:id="rId1"/>
     <sheet name="Do załatwienia" sheetId="2" r:id="rId2"/>
     <sheet name="Do ustalenia" sheetId="3" r:id="rId3"/>
+    <sheet name="Arkusz1" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="114210"/>
+  <calcPr calcId="124519"/>
+  <oleSize ref="A1:N13"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="132">
   <si>
     <t>Pralnia i suszarnia</t>
   </si>
@@ -289,13 +291,136 @@
   </si>
   <si>
     <t>Ocieplenie ścian</t>
+  </si>
+  <si>
+    <t>Węgiel</t>
+  </si>
+  <si>
+    <t>Pompa ciepła</t>
+  </si>
+  <si>
+    <t>Nawiewowe (Rekuperator)</t>
+  </si>
+  <si>
+    <t>Panele słoneczne</t>
+  </si>
+  <si>
+    <t>Drewno</t>
+  </si>
+  <si>
+    <t>Kominkowe</t>
+  </si>
+  <si>
+    <t>Ekogroszek</t>
+  </si>
+  <si>
+    <t>Koszt 1kWh (1)</t>
+  </si>
+  <si>
+    <t>Koszt 1kWh (2)</t>
+  </si>
+  <si>
+    <t>Roczny Kosz ogrzewania 140m2 i wody 300l/d</t>
+  </si>
+  <si>
+    <t>Koszt urządzenia</t>
+  </si>
+  <si>
+    <t>najtańsza 25kW kosztuje 30000</t>
+  </si>
+  <si>
+    <t>Koszt instalacji</t>
+  </si>
+  <si>
+    <t>93000 - http://vikersonn.pl/pompa-ciepla/52.11.200</t>
+  </si>
+  <si>
+    <t>od 40000, centralka 10000</t>
+  </si>
+  <si>
+    <t>Trwałość</t>
+  </si>
+  <si>
+    <t>Bjorn - wieczysta gwarancja (na pompę? Czy instalacje)</t>
+  </si>
+  <si>
+    <t>kilkadziesiąt lat</t>
+  </si>
+  <si>
+    <t>Przegląd</t>
+  </si>
+  <si>
+    <t>Obsługa</t>
+  </si>
+  <si>
+    <t>Bezobsługowa</t>
+  </si>
+  <si>
+    <t>Sterownik</t>
+  </si>
+  <si>
+    <t>Wbudowany w pompe Bjorn</t>
+  </si>
+  <si>
+    <t>Komfort</t>
+  </si>
+  <si>
+    <t>Ogrzewanie podłogowe</t>
+  </si>
+  <si>
+    <t>ok. 150zł/m2</t>
+  </si>
+  <si>
+    <t>czyli</t>
+  </si>
+  <si>
+    <t>Mati</t>
+  </si>
+  <si>
+    <t>wspolczynnik przenikania ciepła</t>
+  </si>
+  <si>
+    <t>W/m2K</t>
+  </si>
+  <si>
+    <t>zapotrzebowanie na ciepla wode</t>
+  </si>
+  <si>
+    <t>kW</t>
+  </si>
+  <si>
+    <t>doba</t>
+  </si>
+  <si>
+    <t>zapotrzebowanie na wode i ogrzewanie</t>
+  </si>
+  <si>
+    <t>zapotrzebowanie gazu na rok na ogrzewanie i c.w.</t>
+  </si>
+  <si>
+    <t>m3/rok</t>
+  </si>
+  <si>
+    <t>Kocioł ok. 10000</t>
+  </si>
+  <si>
+    <t>Trzeba mieć zamknięte okna - do kitu</t>
+  </si>
+  <si>
+    <t>wg opinii: załadunek latem co 14 dni, zima co 3-5 dni</t>
+  </si>
+  <si>
+    <t>jest wybór</t>
+  </si>
+  <si>
+    <t>ok.. 10000 (25kW)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -324,6 +449,15 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="238"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -386,7 +520,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -427,6 +561,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -437,9 +574,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motyw pakietu Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Pakiet Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -477,7 +614,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Pakiet Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -547,7 +684,7 @@
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Pakiet Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -723,7 +860,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:S45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
@@ -1745,4 +1882,469 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:I29"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B2" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="42.5703125" customWidth="1"/>
+    <col min="4" max="4" width="21.5703125" customWidth="1"/>
+    <col min="5" max="5" width="15.5703125" customWidth="1"/>
+    <col min="6" max="6" width="13.42578125" customWidth="1"/>
+    <col min="8" max="8" width="17.28515625" customWidth="1"/>
+    <col min="9" max="9" width="12.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="60">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="B2" s="6">
+        <v>0.17</v>
+      </c>
+      <c r="C2" s="6">
+        <v>0.18</v>
+      </c>
+      <c r="D2" s="6">
+        <v>0.17</v>
+      </c>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="B3" s="6"/>
+      <c r="C3" s="6">
+        <v>0.21</v>
+      </c>
+      <c r="D3" s="6">
+        <v>0.12</v>
+      </c>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6">
+        <v>0.17</v>
+      </c>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6">
+        <v>4500</v>
+      </c>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6">
+        <v>3900</v>
+      </c>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6">
+        <v>3700</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="30">
+      <c r="A5" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="45">
+      <c r="A6" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
+    </row>
+    <row r="7" spans="1:9" ht="45">
+      <c r="A7" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
+    </row>
+    <row r="9" spans="1:9" ht="75">
+      <c r="A9" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="30">
+      <c r="A10" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="45">
+      <c r="A11" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6"/>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+    </row>
+    <row r="13" spans="1:9" ht="30">
+      <c r="A13" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D13" s="1">
+        <f>150*140</f>
+        <v>21000</v>
+      </c>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+    </row>
+    <row r="17" spans="1:9">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+    </row>
+    <row r="18" spans="1:9">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+    </row>
+    <row r="19" spans="1:9">
+      <c r="A19" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+    </row>
+    <row r="20" spans="1:9">
+      <c r="A20" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B20" s="1">
+        <v>0.19</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+    </row>
+    <row r="21" spans="1:9">
+      <c r="A21" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B21" s="1">
+        <v>4.8</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
+    </row>
+    <row r="22" spans="1:9">
+      <c r="A22" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B22" s="1">
+        <v>24</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
+    </row>
+    <row r="23" spans="1:9" ht="30">
+      <c r="A23" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B23" s="1">
+        <v>4275</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
+    </row>
+    <row r="24" spans="1:9">
+      <c r="A24" s="1"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
+    </row>
+    <row r="25" spans="1:9">
+      <c r="A25" s="1"/>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
+      <c r="I25" s="1"/>
+    </row>
+    <row r="26" spans="1:9">
+      <c r="A26" s="22" t="s">
+        <v>97</v>
+      </c>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1"/>
+      <c r="I26" s="1"/>
+    </row>
+    <row r="27" spans="1:9">
+      <c r="A27" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
+      <c r="H27" s="1"/>
+      <c r="I27" s="1"/>
+    </row>
+    <row r="28" spans="1:9">
+      <c r="A28" s="1"/>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
+      <c r="H28" s="1"/>
+      <c r="I28" s="1"/>
+    </row>
+    <row r="29" spans="1:9">
+      <c r="A29" s="1"/>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
+      <c r="H29" s="1"/>
+      <c r="I29" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
kominek i piwnica uzgodnione
</commit_message>
<xml_diff>
--- a/plan/Mati - do uzgodnienia.xlsx
+++ b/plan/Mati - do uzgodnienia.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2505" windowWidth="12540" windowHeight="5940" tabRatio="854" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="2505" windowWidth="12540" windowHeight="5940" tabRatio="854" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Dorady" sheetId="8" r:id="rId1"/>
@@ -12,13 +12,12 @@
     <sheet name="Adaptacja - do uzgodnienia" sheetId="5" r:id="rId3"/>
     <sheet name="Etap budowy - do uzgodnienia" sheetId="6" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="124519"/>
-  <oleSize ref="A1:G14"/>
+  <calcPr calcId="114210"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="118">
   <si>
     <t>Pralnia i suszarnia</t>
   </si>
@@ -378,7 +377,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -405,14 +404,14 @@
     <font>
       <b/>
       <sz val="8"/>
-      <color theme="1"/>
+      <color indexed="8"/>
       <name val="Tahoma"/>
       <family val="2"/>
       <charset val="238"/>
     </font>
     <font>
       <sz val="8"/>
-      <color theme="1"/>
+      <color indexed="8"/>
       <name val="Tahoma"/>
       <family val="2"/>
       <charset val="238"/>
@@ -427,15 +426,21 @@
     <font>
       <b/>
       <sz val="8"/>
-      <color rgb="FFFF0000"/>
+      <color indexed="10"/>
       <name val="Tahoma"/>
       <family val="2"/>
       <charset val="238"/>
     </font>
     <font>
       <sz val="10"/>
-      <color theme="1"/>
+      <color indexed="8"/>
       <name val="Tahoma"/>
+      <family val="2"/>
+      <charset val="238"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="238"/>
     </font>
@@ -449,19 +454,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.499984740745262"/>
+        <fgColor indexed="23"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0"/>
+        <fgColor indexed="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF00CC00"/>
+        <fgColor indexed="11"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -509,19 +514,6 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -537,6 +529,19 @@
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -603,30 +608,30 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -635,18 +640,13 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <mruColors>
-      <color rgb="FF00CC00"/>
-    </mruColors>
-  </colors>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motyw pakietu Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Pakiet Office">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -684,7 +684,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Pakiet Office">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -754,7 +754,7 @@
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Pakiet Office">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1090,6 +1090,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
@@ -1099,7 +1100,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
@@ -1870,6 +1871,7 @@
       <c r="J59" s="13"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="8" type="noConversion"/>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E24">
       <formula1>$Q$2:$Q$6</formula1>
@@ -1884,8 +1886,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:M55"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="10.5"/>
@@ -1947,10 +1949,10 @@
       <c r="G2" s="7"/>
     </row>
     <row r="3" spans="1:13" ht="33">
-      <c r="A3" s="24" t="s">
+      <c r="A3" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="28" t="s">
+      <c r="B3" s="30" t="s">
         <v>37</v>
       </c>
       <c r="C3" s="4" t="s">
@@ -1970,8 +1972,8 @@
       </c>
     </row>
     <row r="4" spans="1:13" ht="22.5">
-      <c r="A4" s="25"/>
-      <c r="B4" s="29"/>
+      <c r="A4" s="27"/>
+      <c r="B4" s="31"/>
       <c r="C4" s="4" t="s">
         <v>45</v>
       </c>
@@ -1989,8 +1991,8 @@
       </c>
     </row>
     <row r="5" spans="1:13" ht="33">
-      <c r="A5" s="26"/>
-      <c r="B5" s="30"/>
+      <c r="A5" s="28"/>
+      <c r="B5" s="32"/>
       <c r="C5" s="4" t="s">
         <v>101</v>
       </c>
@@ -2007,8 +2009,8 @@
       </c>
     </row>
     <row r="6" spans="1:13" ht="22.5">
-      <c r="A6" s="26"/>
-      <c r="B6" s="28" t="s">
+      <c r="A6" s="28"/>
+      <c r="B6" s="30" t="s">
         <v>38</v>
       </c>
       <c r="C6" s="4" t="s">
@@ -2028,8 +2030,8 @@
       </c>
     </row>
     <row r="7" spans="1:13" ht="43.5">
-      <c r="A7" s="26"/>
-      <c r="B7" s="29"/>
+      <c r="A7" s="28"/>
+      <c r="B7" s="31"/>
       <c r="C7" s="4" t="s">
         <v>44</v>
       </c>
@@ -2049,8 +2051,8 @@
       </c>
     </row>
     <row r="8" spans="1:13" ht="21">
-      <c r="A8" s="26"/>
-      <c r="B8" s="29"/>
+      <c r="A8" s="28"/>
+      <c r="B8" s="31"/>
       <c r="C8" s="4" t="s">
         <v>45</v>
       </c>
@@ -2065,8 +2067,8 @@
       </c>
     </row>
     <row r="9" spans="1:13" ht="52.5">
-      <c r="A9" s="26"/>
-      <c r="B9" s="29"/>
+      <c r="A9" s="28"/>
+      <c r="B9" s="31"/>
       <c r="C9" s="4" t="s">
         <v>49</v>
       </c>
@@ -2087,8 +2089,8 @@
       </c>
     </row>
     <row r="10" spans="1:13">
-      <c r="A10" s="26"/>
-      <c r="B10" s="30"/>
+      <c r="A10" s="28"/>
+      <c r="B10" s="32"/>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
@@ -2096,31 +2098,34 @@
       <c r="G10" s="4"/>
     </row>
     <row r="11" spans="1:13" ht="63">
-      <c r="A11" s="26"/>
-      <c r="B11" s="28" t="s">
+      <c r="A11" s="28"/>
+      <c r="B11" s="30" t="s">
         <v>39</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="D11" s="19" t="s">
         <v>98</v>
       </c>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4" t="s">
+      <c r="E11" s="19"/>
+      <c r="F11" s="19" t="s">
         <v>99</v>
       </c>
-      <c r="G11" s="4"/>
-      <c r="I11" s="11" t="s">
+      <c r="G11" s="20"/>
+      <c r="H11" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="J11" s="4" t="s">
+      <c r="I11" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="J11" s="19" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="12" spans="1:13" ht="21">
-      <c r="A12" s="26"/>
-      <c r="B12" s="30"/>
+      <c r="A12" s="28"/>
+      <c r="B12" s="32"/>
       <c r="C12" s="19" t="s">
         <v>48</v>
       </c>
@@ -2137,8 +2142,8 @@
       <c r="J12" s="19"/>
     </row>
     <row r="13" spans="1:13" ht="52.5">
-      <c r="A13" s="26"/>
-      <c r="B13" s="28" t="s">
+      <c r="A13" s="28"/>
+      <c r="B13" s="30" t="s">
         <v>63</v>
       </c>
       <c r="C13" s="4" t="s">
@@ -2155,8 +2160,8 @@
       </c>
     </row>
     <row r="14" spans="1:13">
-      <c r="A14" s="27"/>
-      <c r="B14" s="30"/>
+      <c r="A14" s="29"/>
+      <c r="B14" s="32"/>
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
       <c r="E14" s="4"/>
@@ -2179,7 +2184,7 @@
       <c r="G15" s="4"/>
     </row>
     <row r="16" spans="1:13" ht="31.5">
-      <c r="A16" s="31" t="s">
+      <c r="A16" s="24" t="s">
         <v>31</v>
       </c>
       <c r="B16" s="19" t="s">
@@ -2203,28 +2208,33 @@
       <c r="J16" s="19"/>
     </row>
     <row r="17" spans="1:10" ht="52.5">
-      <c r="A17" s="31"/>
-      <c r="B17" s="4" t="s">
+      <c r="A17" s="24"/>
+      <c r="B17" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="C17" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="D17" s="10" t="s">
+      <c r="D17" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="E17" s="4" t="s">
+      <c r="E17" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="F17" s="10" t="s">
+      <c r="F17" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="G17" s="10" t="s">
+      <c r="G17" s="20" t="s">
         <v>18</v>
       </c>
+      <c r="H17" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="I17" s="19"/>
+      <c r="J17" s="19"/>
     </row>
     <row r="18" spans="1:10" ht="21">
-      <c r="A18" s="31"/>
+      <c r="A18" s="24"/>
       <c r="B18" s="19" t="s">
         <v>32</v>
       </c>
@@ -2240,7 +2250,7 @@
       <c r="J18" s="19"/>
     </row>
     <row r="19" spans="1:10" ht="52.5">
-      <c r="A19" s="32"/>
+      <c r="A19" s="25"/>
       <c r="B19" s="4" t="s">
         <v>33</v>
       </c>
@@ -2659,6 +2669,7 @@
     <mergeCell ref="B11:B12"/>
     <mergeCell ref="B13:B14"/>
   </mergeCells>
+  <phoneticPr fontId="8" type="noConversion"/>
   <dataValidations count="3">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G20 E19:E20 G9 E9">
       <formula1>$Q$2:$Q$7</formula1>
@@ -2683,6 +2694,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
+  <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Instalacje elektryczna - propozycja oświetlenia, gniazdek, włączników
</commit_message>
<xml_diff>
--- a/plan/Mati - do uzgodnienia.xlsx
+++ b/plan/Mati - do uzgodnienia.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2505" windowWidth="17010" windowHeight="5520" tabRatio="854" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="2505" windowWidth="17010" windowHeight="5520" tabRatio="854" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Adaptacja - done" sheetId="5" r:id="rId1"/>
@@ -12,13 +12,14 @@
     <sheet name="Etap budowy SD - uzgodnienia" sheetId="10" r:id="rId3"/>
     <sheet name="Wykończenie - uzgodnienia" sheetId="7" r:id="rId4"/>
     <sheet name="Harmonogram" sheetId="9" r:id="rId5"/>
+    <sheet name="Instalacje - uzgodnienia" sheetId="11" r:id="rId6"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="292">
   <si>
     <t>Piwnica</t>
   </si>
@@ -697,13 +698,218 @@
   </si>
   <si>
     <t>Drzwiczki "ścięty róg" a w środku dwa kosze okrągłe.</t>
+  </si>
+  <si>
+    <t>Zakończenie sprawy RC976</t>
+  </si>
+  <si>
+    <t>Zakończenie sprawy NS912</t>
+  </si>
+  <si>
+    <t>20123-03-01</t>
+  </si>
+  <si>
+    <t>Oświetlenie</t>
+  </si>
+  <si>
+    <t>Pomieszczenie</t>
+  </si>
+  <si>
+    <t>wiatrołap</t>
+  </si>
+  <si>
+    <t>hol</t>
+  </si>
+  <si>
+    <t>kuchnia</t>
+  </si>
+  <si>
+    <t>śpiżarnia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">salon </t>
+  </si>
+  <si>
+    <t>jadalnia</t>
+  </si>
+  <si>
+    <t>gabinet</t>
+  </si>
+  <si>
+    <t>toaleta</t>
+  </si>
+  <si>
+    <t>pom.gosp ogród</t>
+  </si>
+  <si>
+    <t>pom.gosp dom</t>
+  </si>
+  <si>
+    <t>garaż</t>
+  </si>
+  <si>
+    <t>łazienka</t>
+  </si>
+  <si>
+    <t>garderoba</t>
+  </si>
+  <si>
+    <t>pokój 1</t>
+  </si>
+  <si>
+    <t>pokój 2</t>
+  </si>
+  <si>
+    <t>sypialnia</t>
+  </si>
+  <si>
+    <t>jedno główne, sufit</t>
+  </si>
+  <si>
+    <t>jeszcze nie wiem po co, ale pewnie jedno</t>
+  </si>
+  <si>
+    <t>jakieś jedno, np. do odkurzacza?</t>
+  </si>
+  <si>
+    <t>oświetlenie główne-sufit plus oświetlenie blatów (np. halogenki pod szafkami wiszącymi)</t>
+  </si>
+  <si>
+    <t>gniazdka stałe do: lodówki, zmywarki, kuchenki, okapu, mikrofalówki, czajnika
+gniazdko na ścianie koło lodówki, niskie
+gniazdka wolne: po 3 nad blatami (sprzęt: mikser, opiekacz, gofrownica, robot kuchenny, ekspres do kawy</t>
+  </si>
+  <si>
+    <t>oświetlenie główne - sufit lub ściana</t>
+  </si>
+  <si>
+    <t>oświetlenie główne-sufit  
+kinkieciki nad sofą
+kinkieciki na ścianie telewizyjnej</t>
+  </si>
+  <si>
+    <t>INSTALACJA ELEKTRYCZNA</t>
+  </si>
+  <si>
+    <t>dwa podwójne gniazdka na ścianie przy jadalni (za sofą po prawej i po lewej stronie ściany, np. do lampy podłogowej lub ładowarki lub laptopa)
+gniazdka (ok..4szt lub 2sz+listwa) na ścianie telewizyjnej (urządzenia: telewizor, kino domowe, inne)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">oświetlenie główne - sufit  </t>
+  </si>
+  <si>
+    <t>gniazdko na ścianie spiżarni</t>
+  </si>
+  <si>
+    <t>Gniazdka (wg "Budujemy dom" komfortowe jest 1gniazdko/5m2 pomieszczenia)</t>
+  </si>
+  <si>
+    <t>Powierzchnia [m2]</t>
+  </si>
+  <si>
+    <t>korytarz</t>
+  </si>
+  <si>
+    <t>jedno gniazdko? Czy lepiej korzystać z tego w jadalni?</t>
+  </si>
+  <si>
+    <t>klatka schodowa</t>
+  </si>
+  <si>
+    <t>oświetlenie główne - sufit , oświetlenie dodatkowe nad lustrem</t>
+  </si>
+  <si>
+    <t>podwójne gniazdko koło umywalki</t>
+  </si>
+  <si>
+    <t>gniazdko na rekuperator/wentylatory - pod schodami
+gniazdko na pralkę/suszarkę, żelazko, kontroler pieca/zasobnika z wodą</t>
+  </si>
+  <si>
+    <t>oświetlenie punktowe ścienne</t>
+  </si>
+  <si>
+    <t>Włączniki oświetlenia</t>
+  </si>
+  <si>
+    <t>tuż za drzwiami wejściowymi</t>
+  </si>
+  <si>
+    <t>tuż za drzwiami wejściowymi zewnętrznymi (ważniejsze jest, żeby włącznik był bliżej drzwi frontowych niż bliżej drzwi od holu)</t>
+  </si>
+  <si>
+    <t>na ścianie graniczącej z wiatrołapem (albo lepiej na ścianie spiżarki - wtedy będzie po drodze zarówno od holu jak i w drodze do salonu)</t>
+  </si>
+  <si>
+    <t>tuż za drzwiami wejściowymi (zastanawialam się nad włącznikiem na zewnątrz, ale to ryzyko zapomnienie zgaszenia światła po zamknięciu drzwi)</t>
+  </si>
+  <si>
+    <t>na ścianie od klatki schodowej (chociaż co w przypadku wchodzenia do salonu od kuchni?)</t>
+  </si>
+  <si>
+    <t>na ściance zewnętrznej spiżarki (jest dokladnie na drodze salon-kuchnia)</t>
+  </si>
+  <si>
+    <t>tuż za drzwiami wejściowymi od holu (chociaż co w przypadku przechodzenia nocą do garażu? Trzebaby wrócić i zgasić. Drugi włącznik na drzwiach przy garażu? Oświetlenie nie może być czasowe, bo w pom.gosp się robi np. pranie)</t>
+  </si>
+  <si>
+    <t>tuż za drzwiami wejściowymi od garażu (raczej nie będzie się wchodzić nocą z ogrodu, a może? Może lepiej za drzwiami do ogrodu, bo wchodząc od garażu będzie wpadać tam trochę światła garażowego)</t>
+  </si>
+  <si>
+    <t>może jakiś czujnik ruchu? Bo mamy opcje: wjazd samochodem-dom, dom-wyjazd samochodem, dom-ogród, ogród-dom, trzebaby mieć trzy włączniki</t>
+  </si>
+  <si>
+    <t>tuż za drzwiami wejściowymi (zapalić od razu po wejściu, zgasić przy wychodzeniu z domu, czy będzie wygodnie gasić wieczorem przed pójściem na górę? Przed zgaszeniem w holou trzeba bedize przecież zapalić na schodach)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">włącznik1: punkt oświetleniowy korytarzyka do kuchni i korytarzyka do salonu
+</t>
+  </si>
+  <si>
+    <t>gniazdka zwykłe  (wiertarka, sprężarka?, lewarek?) + gniazdko trójfazowe</t>
+  </si>
+  <si>
+    <t>gniazdka zwykłe (kosiarka?, piła?) + gniazdko trójfazowe</t>
+  </si>
+  <si>
+    <t>jedno gniazdko np.. Na półpiętrze? (ale po co?)</t>
+  </si>
+  <si>
+    <t>oświetlenie główne - sufit , oświetlenie nad lustrem, punktowe koło wanny</t>
+  </si>
+  <si>
+    <t>przy schodach</t>
+  </si>
+  <si>
+    <t>oświetlenie główne i punktowe przy wejściu, ośiwetlenie lustra przy lustrze (choociaż, bardzo często zapomina się je zgasić, może zrobić przy wejściu, skoro i tak lustro będzie blisko wejscia)</t>
+  </si>
+  <si>
+    <t>dwa gniazdka koło zlewu (ładowarka do szczoteczki, suszarka, maszynka do golenia), dodatkowe gniazdko na innej ścianie (kryzysowa farelka/depilator)</t>
+  </si>
+  <si>
+    <t>oświetlenie główne - sufit , może jakieś punktowe</t>
+  </si>
+  <si>
+    <t>gniazdka  w okolicy biurka, gniazdko na innej scianie</t>
+  </si>
+  <si>
+    <t>gniazdka koło biurka (komputer, lampka, ładowarka, drukarka, radio), gniazdko na innej scianie</t>
+  </si>
+  <si>
+    <t>po dwa gniazdka po obu stronach łóżka (lampki, ładowarki)</t>
+  </si>
+  <si>
+    <t>PIĘTRO</t>
+  </si>
+  <si>
+    <t>na ściance koło gabinetu (żeby móc właczyć oświetlenie stojąc jeszcze w oświetlonym holu), oraz na górze</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -765,6 +971,15 @@
       <family val="2"/>
       <charset val="238"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -792,7 +1007,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="19">
+  <borders count="22">
     <border>
       <left/>
       <right/>
@@ -1034,11 +1249,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="108">
+  <cellXfs count="121">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1343,6 +1595,25 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -3478,7 +3749,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="J4" sqref="J4:J5"/>
     </sheetView>
@@ -3717,10 +3988,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3790,102 +4061,515 @@
     </row>
     <row r="10" spans="1:4">
       <c r="B10" t="s">
-        <v>118</v>
-      </c>
-      <c r="C10" s="23">
-        <v>41275</v>
-      </c>
+        <v>226</v>
+      </c>
+      <c r="C10" s="23"/>
       <c r="D10" s="23">
-        <v>41306</v>
+        <v>41365</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="B11" t="s">
-        <v>119</v>
-      </c>
-      <c r="C11" s="23">
-        <v>41306</v>
-      </c>
-      <c r="D11" s="23">
-        <v>41320</v>
+        <v>227</v>
+      </c>
+      <c r="C11" s="23"/>
+      <c r="D11" s="23" t="s">
+        <v>228</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="B12" t="s">
-        <v>120</v>
+        <v>118</v>
+      </c>
+      <c r="C12" s="23">
+        <v>41334</v>
       </c>
       <c r="D12" s="23">
-        <v>41334</v>
+        <v>41365</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="B13" t="s">
-        <v>121</v>
+        <v>119</v>
+      </c>
+      <c r="C13" s="23">
+        <v>41365</v>
       </c>
       <c r="D13" s="23">
-        <v>41258</v>
+        <v>41379</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="B14" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D14" s="23">
-        <v>41289</v>
+        <v>41395</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="B15" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D15" s="23">
-        <v>41258</v>
+        <v>41334</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="B16" t="s">
-        <v>124</v>
-      </c>
-      <c r="C16" s="23">
-        <v>41206</v>
+        <v>122</v>
       </c>
       <c r="D16" s="23">
-        <v>41258</v>
+        <v>41379</v>
       </c>
     </row>
     <row r="17" spans="2:4">
       <c r="B17" t="s">
-        <v>125</v>
-      </c>
-      <c r="C17" s="23">
-        <v>41365</v>
+        <v>123</v>
       </c>
       <c r="D17" s="23">
-        <v>41395</v>
+        <v>41320</v>
       </c>
     </row>
     <row r="18" spans="2:4">
       <c r="B18" t="s">
-        <v>126</v>
+        <v>124</v>
+      </c>
+      <c r="C18" s="23">
+        <v>41275</v>
+      </c>
+      <c r="D18" s="23">
+        <v>41320</v>
       </c>
     </row>
     <row r="19" spans="2:4">
       <c r="B19" t="s">
-        <v>127</v>
+        <v>125</v>
+      </c>
+      <c r="C19" s="23">
+        <v>41365</v>
       </c>
       <c r="D19" s="23">
-        <v>41365</v>
+        <v>41395</v>
       </c>
     </row>
     <row r="20" spans="2:4">
       <c r="B20" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4">
+      <c r="B21" t="s">
+        <v>127</v>
+      </c>
+      <c r="D21" s="23">
+        <v>41426</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4">
+      <c r="B22" t="s">
         <v>128</v>
       </c>
-      <c r="D20" s="23">
-        <v>41353</v>
+      <c r="D22" s="23">
+        <v>41414</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="34.140625" customWidth="1"/>
+    <col min="5" max="5" width="45.140625" customWidth="1"/>
+    <col min="6" max="6" width="15.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="15.75" thickBot="1"/>
+    <row r="2" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A2" s="113" t="s">
+        <v>254</v>
+      </c>
+      <c r="B2" s="119"/>
+      <c r="C2" s="114"/>
+      <c r="D2" s="114"/>
+      <c r="E2" s="114"/>
+      <c r="F2" s="115"/>
+    </row>
+    <row r="3" spans="1:6" ht="30">
+      <c r="A3" s="116" t="s">
+        <v>230</v>
+      </c>
+      <c r="B3" s="116" t="s">
+        <v>259</v>
+      </c>
+      <c r="C3" s="117" t="s">
+        <v>229</v>
+      </c>
+      <c r="D3" s="117" t="s">
+        <v>267</v>
+      </c>
+      <c r="E3" s="117" t="s">
+        <v>258</v>
+      </c>
+      <c r="F3" s="112" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="60">
+      <c r="A4" s="118" t="s">
+        <v>231</v>
+      </c>
+      <c r="B4" s="120">
+        <v>3.36</v>
+      </c>
+      <c r="C4" s="110" t="s">
+        <v>247</v>
+      </c>
+      <c r="D4" s="110" t="s">
+        <v>269</v>
+      </c>
+      <c r="E4" s="110" t="s">
+        <v>248</v>
+      </c>
+      <c r="F4" s="111"/>
+    </row>
+    <row r="5" spans="1:6" ht="105">
+      <c r="A5" s="118" t="s">
+        <v>232</v>
+      </c>
+      <c r="B5" s="120">
+        <v>14.54</v>
+      </c>
+      <c r="C5" s="110" t="s">
+        <v>278</v>
+      </c>
+      <c r="D5" s="110" t="s">
+        <v>277</v>
+      </c>
+      <c r="E5" s="110" t="s">
+        <v>249</v>
+      </c>
+      <c r="F5" s="111"/>
+    </row>
+    <row r="6" spans="1:6" ht="90">
+      <c r="A6" s="118" t="s">
+        <v>233</v>
+      </c>
+      <c r="B6" s="120">
+        <v>8.34</v>
+      </c>
+      <c r="C6" s="110" t="s">
+        <v>250</v>
+      </c>
+      <c r="D6" s="110" t="s">
+        <v>270</v>
+      </c>
+      <c r="E6" s="110" t="s">
+        <v>251</v>
+      </c>
+      <c r="F6" s="111"/>
+    </row>
+    <row r="7" spans="1:6" ht="75">
+      <c r="A7" s="118" t="s">
+        <v>234</v>
+      </c>
+      <c r="B7" s="120">
+        <v>1.71</v>
+      </c>
+      <c r="C7" s="110" t="s">
+        <v>252</v>
+      </c>
+      <c r="D7" s="110" t="s">
+        <v>271</v>
+      </c>
+      <c r="E7" s="110" t="s">
+        <v>261</v>
+      </c>
+      <c r="F7" s="111"/>
+    </row>
+    <row r="8" spans="1:6" ht="90">
+      <c r="A8" s="118" t="s">
+        <v>235</v>
+      </c>
+      <c r="B8" s="120">
+        <v>20</v>
+      </c>
+      <c r="C8" s="110" t="s">
+        <v>253</v>
+      </c>
+      <c r="D8" s="110" t="s">
+        <v>272</v>
+      </c>
+      <c r="E8" s="110" t="s">
+        <v>255</v>
+      </c>
+      <c r="F8" s="111"/>
+    </row>
+    <row r="9" spans="1:6" ht="30">
+      <c r="A9" s="118" t="s">
+        <v>236</v>
+      </c>
+      <c r="B9" s="120">
+        <v>9</v>
+      </c>
+      <c r="C9" s="110" t="s">
+        <v>256</v>
+      </c>
+      <c r="D9" s="110" t="s">
+        <v>273</v>
+      </c>
+      <c r="E9" s="110" t="s">
+        <v>257</v>
+      </c>
+      <c r="F9" s="111"/>
+    </row>
+    <row r="10" spans="1:6" ht="30">
+      <c r="A10" s="118" t="s">
+        <v>237</v>
+      </c>
+      <c r="B10" s="120">
+        <v>11.26</v>
+      </c>
+      <c r="C10" s="110" t="s">
+        <v>256</v>
+      </c>
+      <c r="D10" s="110" t="s">
+        <v>268</v>
+      </c>
+      <c r="E10" s="110" t="s">
+        <v>287</v>
+      </c>
+      <c r="F10" s="111"/>
+    </row>
+    <row r="11" spans="1:6" ht="30">
+      <c r="A11" s="118" t="s">
+        <v>238</v>
+      </c>
+      <c r="B11" s="120">
+        <v>2.72</v>
+      </c>
+      <c r="C11" s="110" t="s">
+        <v>263</v>
+      </c>
+      <c r="D11" s="110" t="s">
+        <v>268</v>
+      </c>
+      <c r="E11" s="110" t="s">
+        <v>264</v>
+      </c>
+      <c r="F11" s="111"/>
+    </row>
+    <row r="12" spans="1:6" ht="105">
+      <c r="A12" s="118" t="s">
+        <v>240</v>
+      </c>
+      <c r="B12" s="120">
+        <v>10.66</v>
+      </c>
+      <c r="C12" s="110" t="s">
+        <v>256</v>
+      </c>
+      <c r="D12" s="110" t="s">
+        <v>274</v>
+      </c>
+      <c r="E12" s="110" t="s">
+        <v>265</v>
+      </c>
+      <c r="F12" s="111"/>
+    </row>
+    <row r="13" spans="1:6" ht="105">
+      <c r="A13" s="118" t="s">
+        <v>239</v>
+      </c>
+      <c r="B13" s="120">
+        <v>5.33</v>
+      </c>
+      <c r="C13" s="110" t="s">
+        <v>256</v>
+      </c>
+      <c r="D13" s="110" t="s">
+        <v>275</v>
+      </c>
+      <c r="E13" s="110" t="s">
+        <v>280</v>
+      </c>
+      <c r="F13" s="111"/>
+    </row>
+    <row r="14" spans="1:6" ht="75">
+      <c r="A14" s="118" t="s">
+        <v>241</v>
+      </c>
+      <c r="B14" s="120">
+        <v>19.329999999999998</v>
+      </c>
+      <c r="C14" s="110" t="s">
+        <v>256</v>
+      </c>
+      <c r="D14" s="110" t="s">
+        <v>276</v>
+      </c>
+      <c r="E14" s="110" t="s">
+        <v>279</v>
+      </c>
+      <c r="F14" s="111"/>
+    </row>
+    <row r="15" spans="1:6" ht="45">
+      <c r="A15" s="118" t="s">
+        <v>262</v>
+      </c>
+      <c r="B15" s="120"/>
+      <c r="C15" s="110" t="s">
+        <v>266</v>
+      </c>
+      <c r="D15" s="110" t="s">
+        <v>291</v>
+      </c>
+      <c r="E15" s="110" t="s">
+        <v>281</v>
+      </c>
+      <c r="F15" s="111"/>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="118" t="s">
+        <v>290</v>
+      </c>
+      <c r="B16" s="120"/>
+      <c r="C16" s="110"/>
+      <c r="D16" s="110"/>
+      <c r="E16" s="110"/>
+      <c r="F16" s="111"/>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="118" t="s">
+        <v>260</v>
+      </c>
+      <c r="B17" s="120">
+        <v>5.52</v>
+      </c>
+      <c r="C17" s="110" t="s">
+        <v>256</v>
+      </c>
+      <c r="D17" s="110" t="s">
+        <v>283</v>
+      </c>
+      <c r="E17" s="110"/>
+      <c r="F17" s="111"/>
+    </row>
+    <row r="18" spans="1:6" ht="90">
+      <c r="A18" s="118" t="s">
+        <v>242</v>
+      </c>
+      <c r="B18" s="120">
+        <v>7.89</v>
+      </c>
+      <c r="C18" s="110" t="s">
+        <v>282</v>
+      </c>
+      <c r="D18" s="110" t="s">
+        <v>284</v>
+      </c>
+      <c r="E18" s="110" t="s">
+        <v>285</v>
+      </c>
+      <c r="F18" s="111"/>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" s="118" t="s">
+        <v>243</v>
+      </c>
+      <c r="B19" s="120">
+        <v>3.2</v>
+      </c>
+      <c r="C19" s="110" t="s">
+        <v>256</v>
+      </c>
+      <c r="D19" s="110" t="s">
+        <v>268</v>
+      </c>
+      <c r="E19" s="110"/>
+      <c r="F19" s="111"/>
+    </row>
+    <row r="20" spans="1:6" ht="45">
+      <c r="A20" s="118" t="s">
+        <v>244</v>
+      </c>
+      <c r="B20" s="120">
+        <v>11.14</v>
+      </c>
+      <c r="C20" s="110" t="s">
+        <v>256</v>
+      </c>
+      <c r="D20" s="110" t="s">
+        <v>268</v>
+      </c>
+      <c r="E20" s="110" t="s">
+        <v>288</v>
+      </c>
+      <c r="F20" s="111"/>
+    </row>
+    <row r="21" spans="1:6" ht="45">
+      <c r="A21" s="118" t="s">
+        <v>245</v>
+      </c>
+      <c r="B21" s="120">
+        <v>11.59</v>
+      </c>
+      <c r="C21" s="110" t="s">
+        <v>256</v>
+      </c>
+      <c r="D21" s="110" t="s">
+        <v>268</v>
+      </c>
+      <c r="E21" s="110" t="s">
+        <v>288</v>
+      </c>
+      <c r="F21" s="111"/>
+    </row>
+    <row r="22" spans="1:6" ht="30">
+      <c r="A22" s="118" t="s">
+        <v>246</v>
+      </c>
+      <c r="B22" s="120">
+        <v>13.8</v>
+      </c>
+      <c r="C22" s="110" t="s">
+        <v>286</v>
+      </c>
+      <c r="D22" s="110" t="s">
+        <v>268</v>
+      </c>
+      <c r="E22" s="110" t="s">
+        <v>289</v>
+      </c>
+      <c r="F22" s="109"/>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="C23" s="108"/>
+      <c r="D23" s="108"/>
+      <c r="E23" s="108"/>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="C24" s="108"/>
+      <c r="D24" s="108"/>
+      <c r="E24" s="108"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A2:F2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
instalacja elektryczna - cd
</commit_message>
<xml_diff>
--- a/plan/Mati - do uzgodnienia.xlsx
+++ b/plan/Mati - do uzgodnienia.xlsx
@@ -1550,51 +1550,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1604,16 +1559,61 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -1969,7 +1969,7 @@
       <c r="L1" s="4"/>
     </row>
     <row r="2" spans="1:12" ht="52.5">
-      <c r="A2" s="93" t="s">
+      <c r="A2" s="102" t="s">
         <v>25</v>
       </c>
       <c r="B2" s="67" t="s">
@@ -1997,7 +1997,7 @@
       </c>
     </row>
     <row r="3" spans="1:12" ht="126">
-      <c r="A3" s="93"/>
+      <c r="A3" s="102"/>
       <c r="B3" s="67" t="s">
         <v>26</v>
       </c>
@@ -2031,7 +2031,7 @@
       <c r="J4" s="81"/>
     </row>
     <row r="5" spans="1:12" ht="31.5">
-      <c r="A5" s="94" t="s">
+      <c r="A5" s="103" t="s">
         <v>24</v>
       </c>
       <c r="B5" s="67" t="s">
@@ -2049,7 +2049,7 @@
       <c r="J5" s="81"/>
     </row>
     <row r="6" spans="1:12" ht="21">
-      <c r="A6" s="93"/>
+      <c r="A6" s="102"/>
       <c r="B6" s="67" t="s">
         <v>9</v>
       </c>
@@ -2069,7 +2069,7 @@
       <c r="J6" s="81"/>
     </row>
     <row r="7" spans="1:12" ht="21">
-      <c r="A7" s="93"/>
+      <c r="A7" s="102"/>
       <c r="B7" s="67" t="s">
         <v>10</v>
       </c>
@@ -2089,7 +2089,7 @@
       <c r="J7" s="81"/>
     </row>
     <row r="8" spans="1:12" ht="21">
-      <c r="A8" s="93"/>
+      <c r="A8" s="102"/>
       <c r="B8" s="67" t="s">
         <v>12</v>
       </c>
@@ -2109,7 +2109,7 @@
       <c r="J8" s="81"/>
     </row>
     <row r="9" spans="1:12" ht="21">
-      <c r="A9" s="95"/>
+      <c r="A9" s="104"/>
       <c r="B9" s="67" t="s">
         <v>8</v>
       </c>
@@ -2476,7 +2476,7 @@
       </c>
     </row>
     <row r="2" spans="1:12" ht="15">
-      <c r="A2" s="96" t="s">
+      <c r="A2" s="105" t="s">
         <v>107</v>
       </c>
       <c r="B2" s="33" t="s">
@@ -2497,7 +2497,7 @@
       </c>
     </row>
     <row r="3" spans="1:12" ht="85.5">
-      <c r="A3" s="97"/>
+      <c r="A3" s="106"/>
       <c r="B3" s="46" t="s">
         <v>56</v>
       </c>
@@ -2516,7 +2516,7 @@
       <c r="L3"/>
     </row>
     <row r="4" spans="1:12" ht="17.25" customHeight="1" thickBot="1">
-      <c r="A4" s="98"/>
+      <c r="A4" s="107"/>
       <c r="B4" s="45" t="s">
         <v>97</v>
       </c>
@@ -2535,7 +2535,7 @@
       </c>
     </row>
     <row r="5" spans="1:12" ht="15">
-      <c r="A5" s="99" t="s">
+      <c r="A5" s="108" t="s">
         <v>99</v>
       </c>
       <c r="B5" s="62" t="s">
@@ -2562,7 +2562,7 @@
       </c>
     </row>
     <row r="6" spans="1:12" ht="33">
-      <c r="A6" s="100"/>
+      <c r="A6" s="109"/>
       <c r="B6" s="43" t="s">
         <v>135</v>
       </c>
@@ -2581,7 +2581,7 @@
       <c r="L6"/>
     </row>
     <row r="7" spans="1:12" ht="22.5">
-      <c r="A7" s="100"/>
+      <c r="A7" s="109"/>
       <c r="B7" s="39" t="s">
         <v>73</v>
       </c>
@@ -2608,7 +2608,7 @@
       </c>
     </row>
     <row r="8" spans="1:12" ht="33">
-      <c r="A8" s="100"/>
+      <c r="A8" s="109"/>
       <c r="B8" s="39" t="s">
         <v>74</v>
       </c>
@@ -2629,7 +2629,7 @@
       </c>
     </row>
     <row r="9" spans="1:12" ht="52.5">
-      <c r="A9" s="100"/>
+      <c r="A9" s="109"/>
       <c r="B9" s="67" t="s">
         <v>91</v>
       </c>
@@ -2647,7 +2647,7 @@
       </c>
     </row>
     <row r="10" spans="1:12" ht="21">
-      <c r="A10" s="100"/>
+      <c r="A10" s="109"/>
       <c r="B10" s="67" t="s">
         <v>76</v>
       </c>
@@ -2665,8 +2665,8 @@
       </c>
     </row>
     <row r="11" spans="1:12" ht="31.5">
-      <c r="A11" s="100"/>
-      <c r="B11" s="101" t="s">
+      <c r="A11" s="109"/>
+      <c r="B11" s="110" t="s">
         <v>138</v>
       </c>
       <c r="C11" s="68" t="s">
@@ -2683,8 +2683,8 @@
       </c>
     </row>
     <row r="12" spans="1:12" ht="21">
-      <c r="A12" s="100"/>
-      <c r="B12" s="103"/>
+      <c r="A12" s="109"/>
+      <c r="B12" s="112"/>
       <c r="C12" s="68" t="s">
         <v>143</v>
       </c>
@@ -2699,8 +2699,8 @@
       </c>
     </row>
     <row r="13" spans="1:12" ht="31.5">
-      <c r="A13" s="100"/>
-      <c r="B13" s="102"/>
+      <c r="A13" s="109"/>
+      <c r="B13" s="111"/>
       <c r="C13" s="17" t="s">
         <v>144</v>
       </c>
@@ -2713,7 +2713,7 @@
       <c r="J13" s="19"/>
     </row>
     <row r="14" spans="1:12">
-      <c r="A14" s="100"/>
+      <c r="A14" s="109"/>
       <c r="B14" s="39" t="s">
         <v>84</v>
       </c>
@@ -2729,8 +2729,8 @@
       <c r="J14" s="19"/>
     </row>
     <row r="15" spans="1:12" ht="42">
-      <c r="A15" s="100"/>
-      <c r="B15" s="101" t="s">
+      <c r="A15" s="109"/>
+      <c r="B15" s="110" t="s">
         <v>140</v>
       </c>
       <c r="C15" s="17" t="s">
@@ -2745,8 +2745,8 @@
       <c r="J15" s="19"/>
     </row>
     <row r="16" spans="1:12" ht="21">
-      <c r="A16" s="100"/>
-      <c r="B16" s="102"/>
+      <c r="A16" s="109"/>
+      <c r="B16" s="111"/>
       <c r="C16" s="9" t="s">
         <v>172</v>
       </c>
@@ -2763,7 +2763,7 @@
       <c r="J16" s="57"/>
     </row>
     <row r="17" spans="1:11" ht="31.5">
-      <c r="A17" s="100"/>
+      <c r="A17" s="109"/>
       <c r="B17" s="44" t="s">
         <v>97</v>
       </c>
@@ -2789,7 +2789,7 @@
       <c r="J17" s="58"/>
     </row>
     <row r="18" spans="1:11">
-      <c r="A18" s="100"/>
+      <c r="A18" s="109"/>
       <c r="B18" s="44" t="s">
         <v>100</v>
       </c>
@@ -2805,7 +2805,7 @@
       <c r="J18" s="22"/>
     </row>
     <row r="19" spans="1:11">
-      <c r="A19" s="100"/>
+      <c r="A19" s="109"/>
       <c r="B19" s="44" t="s">
         <v>105</v>
       </c>
@@ -2821,7 +2821,7 @@
       <c r="J19" s="22"/>
     </row>
     <row r="20" spans="1:11" ht="31.5">
-      <c r="A20" s="100"/>
+      <c r="A20" s="109"/>
       <c r="B20" s="44" t="s">
         <v>103</v>
       </c>
@@ -2837,7 +2837,7 @@
       <c r="J20" s="11"/>
     </row>
     <row r="21" spans="1:11" ht="42.75" thickBot="1">
-      <c r="A21" s="98"/>
+      <c r="A21" s="107"/>
       <c r="B21" s="45" t="s">
         <v>104</v>
       </c>
@@ -2857,7 +2857,7 @@
       <c r="J21" s="14"/>
     </row>
     <row r="22" spans="1:11">
-      <c r="A22" s="99" t="s">
+      <c r="A22" s="108" t="s">
         <v>64</v>
       </c>
       <c r="B22" s="62" t="s">
@@ -2877,7 +2877,7 @@
       </c>
     </row>
     <row r="23" spans="1:11" ht="31.5">
-      <c r="A23" s="100"/>
+      <c r="A23" s="109"/>
       <c r="B23" s="75" t="s">
         <v>68</v>
       </c>
@@ -2899,7 +2899,7 @@
       </c>
     </row>
     <row r="24" spans="1:11" ht="63">
-      <c r="A24" s="100"/>
+      <c r="A24" s="109"/>
       <c r="B24" s="44" t="s">
         <v>101</v>
       </c>
@@ -2917,7 +2917,7 @@
       <c r="J24" s="22"/>
     </row>
     <row r="25" spans="1:11" ht="11.25" thickBot="1">
-      <c r="A25" s="98"/>
+      <c r="A25" s="107"/>
       <c r="B25" s="45" t="s">
         <v>97</v>
       </c>
@@ -3430,10 +3430,10 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="31.5">
-      <c r="A2" s="104" t="s">
+      <c r="A2" s="113" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="105" t="s">
+      <c r="B2" s="114" t="s">
         <v>96</v>
       </c>
       <c r="C2" s="24" t="s">
@@ -3452,8 +3452,8 @@
       <c r="J2" s="24"/>
     </row>
     <row r="3" spans="1:10" ht="31.5">
-      <c r="A3" s="104"/>
-      <c r="B3" s="105"/>
+      <c r="A3" s="113"/>
+      <c r="B3" s="114"/>
       <c r="C3" s="24" t="s">
         <v>131</v>
       </c>
@@ -3470,7 +3470,7 @@
       <c r="J3" s="24"/>
     </row>
     <row r="4" spans="1:10" ht="42">
-      <c r="A4" s="104" t="s">
+      <c r="A4" s="113" t="s">
         <v>157</v>
       </c>
       <c r="B4" s="37" t="s">
@@ -3490,7 +3490,7 @@
       <c r="J4" s="24"/>
     </row>
     <row r="5" spans="1:10">
-      <c r="A5" s="104"/>
+      <c r="A5" s="113"/>
       <c r="B5" s="82" t="s">
         <v>159</v>
       </c>
@@ -3510,8 +3510,8 @@
       <c r="J5" s="84"/>
     </row>
     <row r="6" spans="1:10" ht="73.5">
-      <c r="A6" s="104"/>
-      <c r="B6" s="105" t="s">
+      <c r="A6" s="113"/>
+      <c r="B6" s="114" t="s">
         <v>34</v>
       </c>
       <c r="C6" s="27" t="s">
@@ -3534,8 +3534,8 @@
       <c r="J6" s="27"/>
     </row>
     <row r="7" spans="1:10" ht="42">
-      <c r="A7" s="104"/>
-      <c r="B7" s="105"/>
+      <c r="A7" s="113"/>
+      <c r="B7" s="114"/>
       <c r="C7" s="83" t="s">
         <v>88</v>
       </c>
@@ -3554,8 +3554,8 @@
       </c>
     </row>
     <row r="8" spans="1:10" ht="42.75" thickBot="1">
-      <c r="A8" s="104"/>
-      <c r="B8" s="106" t="s">
+      <c r="A8" s="113"/>
+      <c r="B8" s="115" t="s">
         <v>29</v>
       </c>
       <c r="C8" s="2" t="s">
@@ -3578,8 +3578,8 @@
       <c r="J8" s="2"/>
     </row>
     <row r="9" spans="1:10" ht="31.5">
-      <c r="A9" s="104"/>
-      <c r="B9" s="106"/>
+      <c r="A9" s="113"/>
+      <c r="B9" s="115"/>
       <c r="C9" s="62" t="s">
         <v>33</v>
       </c>
@@ -3596,7 +3596,7 @@
       </c>
     </row>
     <row r="10" spans="1:10" ht="52.5">
-      <c r="A10" s="104" t="s">
+      <c r="A10" s="113" t="s">
         <v>160</v>
       </c>
       <c r="B10" s="37" t="s">
@@ -3614,7 +3614,7 @@
       <c r="J10" s="27"/>
     </row>
     <row r="11" spans="1:10" ht="52.5">
-      <c r="A11" s="104"/>
+      <c r="A11" s="113"/>
       <c r="B11" s="67" t="s">
         <v>169</v>
       </c>
@@ -3640,7 +3640,7 @@
       </c>
     </row>
     <row r="12" spans="1:10" ht="41.25" customHeight="1">
-      <c r="A12" s="104"/>
+      <c r="A12" s="113"/>
       <c r="B12" s="67" t="s">
         <v>168</v>
       </c>
@@ -3815,7 +3815,7 @@
       </c>
     </row>
     <row r="3" spans="1:10" ht="52.5">
-      <c r="A3" s="107" t="s">
+      <c r="A3" s="116" t="s">
         <v>176</v>
       </c>
       <c r="B3" s="86" t="s">
@@ -3837,7 +3837,7 @@
       </c>
     </row>
     <row r="4" spans="1:10" ht="31.5">
-      <c r="A4" s="107"/>
+      <c r="A4" s="116"/>
       <c r="B4" s="86" t="s">
         <v>180</v>
       </c>
@@ -3859,7 +3859,7 @@
       </c>
     </row>
     <row r="5" spans="1:10" ht="21">
-      <c r="A5" s="107"/>
+      <c r="A5" s="116"/>
       <c r="B5" s="86" t="s">
         <v>223</v>
       </c>
@@ -3879,7 +3879,7 @@
       </c>
     </row>
     <row r="6" spans="1:10" ht="52.5">
-      <c r="A6" s="107"/>
+      <c r="A6" s="116"/>
       <c r="B6" s="86" t="s">
         <v>181</v>
       </c>
@@ -4183,8 +4183,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4198,372 +4198,372 @@
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" thickBot="1"/>
     <row r="2" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A2" s="113" t="s">
+      <c r="A2" s="117" t="s">
         <v>254</v>
       </c>
-      <c r="B2" s="119"/>
-      <c r="C2" s="114"/>
-      <c r="D2" s="114"/>
-      <c r="E2" s="114"/>
-      <c r="F2" s="115"/>
+      <c r="B2" s="118"/>
+      <c r="C2" s="119"/>
+      <c r="D2" s="119"/>
+      <c r="E2" s="119"/>
+      <c r="F2" s="120"/>
     </row>
     <row r="3" spans="1:6" ht="30">
-      <c r="A3" s="116" t="s">
+      <c r="A3" s="98" t="s">
         <v>230</v>
       </c>
-      <c r="B3" s="116" t="s">
+      <c r="B3" s="98" t="s">
         <v>259</v>
       </c>
-      <c r="C3" s="117" t="s">
+      <c r="C3" s="99" t="s">
         <v>229</v>
       </c>
-      <c r="D3" s="117" t="s">
+      <c r="D3" s="99" t="s">
         <v>267</v>
       </c>
-      <c r="E3" s="117" t="s">
+      <c r="E3" s="99" t="s">
         <v>258</v>
       </c>
-      <c r="F3" s="112" t="s">
+      <c r="F3" s="97" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="60">
-      <c r="A4" s="118" t="s">
+      <c r="A4" s="100" t="s">
         <v>231</v>
       </c>
-      <c r="B4" s="120">
+      <c r="B4" s="101">
         <v>3.36</v>
       </c>
-      <c r="C4" s="110" t="s">
+      <c r="C4" s="95" t="s">
         <v>247</v>
       </c>
-      <c r="D4" s="110" t="s">
+      <c r="D4" s="95" t="s">
         <v>269</v>
       </c>
-      <c r="E4" s="110" t="s">
+      <c r="E4" s="95" t="s">
         <v>248</v>
       </c>
-      <c r="F4" s="111"/>
+      <c r="F4" s="96"/>
     </row>
     <row r="5" spans="1:6" ht="105">
-      <c r="A5" s="118" t="s">
+      <c r="A5" s="100" t="s">
         <v>232</v>
       </c>
-      <c r="B5" s="120">
+      <c r="B5" s="101">
         <v>14.54</v>
       </c>
-      <c r="C5" s="110" t="s">
+      <c r="C5" s="95" t="s">
         <v>278</v>
       </c>
-      <c r="D5" s="110" t="s">
+      <c r="D5" s="95" t="s">
         <v>277</v>
       </c>
-      <c r="E5" s="110" t="s">
+      <c r="E5" s="95" t="s">
         <v>249</v>
       </c>
-      <c r="F5" s="111"/>
+      <c r="F5" s="96"/>
     </row>
     <row r="6" spans="1:6" ht="90">
-      <c r="A6" s="118" t="s">
+      <c r="A6" s="100" t="s">
         <v>233</v>
       </c>
-      <c r="B6" s="120">
+      <c r="B6" s="101">
         <v>8.34</v>
       </c>
-      <c r="C6" s="110" t="s">
+      <c r="C6" s="95" t="s">
         <v>250</v>
       </c>
-      <c r="D6" s="110" t="s">
+      <c r="D6" s="95" t="s">
         <v>270</v>
       </c>
-      <c r="E6" s="110" t="s">
+      <c r="E6" s="95" t="s">
         <v>251</v>
       </c>
-      <c r="F6" s="111"/>
+      <c r="F6" s="96"/>
     </row>
     <row r="7" spans="1:6" ht="75">
-      <c r="A7" s="118" t="s">
+      <c r="A7" s="100" t="s">
         <v>234</v>
       </c>
-      <c r="B7" s="120">
+      <c r="B7" s="101">
         <v>1.71</v>
       </c>
-      <c r="C7" s="110" t="s">
+      <c r="C7" s="95" t="s">
         <v>252</v>
       </c>
-      <c r="D7" s="110" t="s">
+      <c r="D7" s="95" t="s">
         <v>271</v>
       </c>
-      <c r="E7" s="110" t="s">
+      <c r="E7" s="95" t="s">
         <v>261</v>
       </c>
-      <c r="F7" s="111"/>
+      <c r="F7" s="96"/>
     </row>
     <row r="8" spans="1:6" ht="90">
-      <c r="A8" s="118" t="s">
+      <c r="A8" s="100" t="s">
         <v>235</v>
       </c>
-      <c r="B8" s="120">
+      <c r="B8" s="101">
         <v>20</v>
       </c>
-      <c r="C8" s="110" t="s">
+      <c r="C8" s="95" t="s">
         <v>253</v>
       </c>
-      <c r="D8" s="110" t="s">
+      <c r="D8" s="95" t="s">
         <v>272</v>
       </c>
-      <c r="E8" s="110" t="s">
+      <c r="E8" s="95" t="s">
         <v>255</v>
       </c>
-      <c r="F8" s="111"/>
+      <c r="F8" s="96"/>
     </row>
     <row r="9" spans="1:6" ht="30">
-      <c r="A9" s="118" t="s">
+      <c r="A9" s="100" t="s">
         <v>236</v>
       </c>
-      <c r="B9" s="120">
+      <c r="B9" s="101">
         <v>9</v>
       </c>
-      <c r="C9" s="110" t="s">
+      <c r="C9" s="95" t="s">
         <v>256</v>
       </c>
-      <c r="D9" s="110" t="s">
+      <c r="D9" s="95" t="s">
         <v>273</v>
       </c>
-      <c r="E9" s="110" t="s">
+      <c r="E9" s="95" t="s">
         <v>257</v>
       </c>
-      <c r="F9" s="111"/>
+      <c r="F9" s="96"/>
     </row>
     <row r="10" spans="1:6" ht="30">
-      <c r="A10" s="118" t="s">
+      <c r="A10" s="100" t="s">
         <v>237</v>
       </c>
-      <c r="B10" s="120">
+      <c r="B10" s="101">
         <v>11.26</v>
       </c>
-      <c r="C10" s="110" t="s">
+      <c r="C10" s="95" t="s">
         <v>256</v>
       </c>
-      <c r="D10" s="110" t="s">
+      <c r="D10" s="95" t="s">
         <v>268</v>
       </c>
-      <c r="E10" s="110" t="s">
+      <c r="E10" s="95" t="s">
         <v>287</v>
       </c>
-      <c r="F10" s="111"/>
+      <c r="F10" s="96"/>
     </row>
     <row r="11" spans="1:6" ht="30">
-      <c r="A11" s="118" t="s">
+      <c r="A11" s="100" t="s">
         <v>238</v>
       </c>
-      <c r="B11" s="120">
+      <c r="B11" s="101">
         <v>2.72</v>
       </c>
-      <c r="C11" s="110" t="s">
+      <c r="C11" s="95" t="s">
         <v>263</v>
       </c>
-      <c r="D11" s="110" t="s">
+      <c r="D11" s="95" t="s">
         <v>268</v>
       </c>
-      <c r="E11" s="110" t="s">
+      <c r="E11" s="95" t="s">
         <v>264</v>
       </c>
-      <c r="F11" s="111"/>
+      <c r="F11" s="96"/>
     </row>
     <row r="12" spans="1:6" ht="105">
-      <c r="A12" s="118" t="s">
+      <c r="A12" s="100" t="s">
         <v>240</v>
       </c>
-      <c r="B12" s="120">
+      <c r="B12" s="101">
         <v>10.66</v>
       </c>
-      <c r="C12" s="110" t="s">
+      <c r="C12" s="95" t="s">
         <v>256</v>
       </c>
-      <c r="D12" s="110" t="s">
+      <c r="D12" s="95" t="s">
         <v>274</v>
       </c>
-      <c r="E12" s="110" t="s">
+      <c r="E12" s="95" t="s">
         <v>265</v>
       </c>
-      <c r="F12" s="111"/>
+      <c r="F12" s="96"/>
     </row>
     <row r="13" spans="1:6" ht="105">
-      <c r="A13" s="118" t="s">
+      <c r="A13" s="100" t="s">
         <v>239</v>
       </c>
-      <c r="B13" s="120">
+      <c r="B13" s="101">
         <v>5.33</v>
       </c>
-      <c r="C13" s="110" t="s">
+      <c r="C13" s="95" t="s">
         <v>256</v>
       </c>
-      <c r="D13" s="110" t="s">
+      <c r="D13" s="95" t="s">
         <v>275</v>
       </c>
-      <c r="E13" s="110" t="s">
+      <c r="E13" s="95" t="s">
         <v>280</v>
       </c>
-      <c r="F13" s="111"/>
+      <c r="F13" s="96"/>
     </row>
     <row r="14" spans="1:6" ht="75">
-      <c r="A14" s="118" t="s">
+      <c r="A14" s="100" t="s">
         <v>241</v>
       </c>
-      <c r="B14" s="120">
+      <c r="B14" s="101">
         <v>19.329999999999998</v>
       </c>
-      <c r="C14" s="110" t="s">
+      <c r="C14" s="95" t="s">
         <v>256</v>
       </c>
-      <c r="D14" s="110" t="s">
+      <c r="D14" s="95" t="s">
         <v>276</v>
       </c>
-      <c r="E14" s="110" t="s">
+      <c r="E14" s="95" t="s">
         <v>279</v>
       </c>
-      <c r="F14" s="111"/>
+      <c r="F14" s="96"/>
     </row>
     <row r="15" spans="1:6" ht="45">
-      <c r="A15" s="118" t="s">
+      <c r="A15" s="100" t="s">
         <v>262</v>
       </c>
-      <c r="B15" s="120"/>
-      <c r="C15" s="110" t="s">
+      <c r="B15" s="101"/>
+      <c r="C15" s="95" t="s">
         <v>266</v>
       </c>
-      <c r="D15" s="110" t="s">
+      <c r="D15" s="95" t="s">
         <v>291</v>
       </c>
-      <c r="E15" s="110" t="s">
+      <c r="E15" s="95" t="s">
         <v>281</v>
       </c>
-      <c r="F15" s="111"/>
+      <c r="F15" s="96"/>
     </row>
     <row r="16" spans="1:6">
-      <c r="A16" s="118" t="s">
+      <c r="A16" s="100" t="s">
         <v>290</v>
       </c>
-      <c r="B16" s="120"/>
-      <c r="C16" s="110"/>
-      <c r="D16" s="110"/>
-      <c r="E16" s="110"/>
-      <c r="F16" s="111"/>
+      <c r="B16" s="101"/>
+      <c r="C16" s="95"/>
+      <c r="D16" s="95"/>
+      <c r="E16" s="95"/>
+      <c r="F16" s="96"/>
     </row>
     <row r="17" spans="1:6">
-      <c r="A17" s="118" t="s">
+      <c r="A17" s="100" t="s">
         <v>260</v>
       </c>
-      <c r="B17" s="120">
+      <c r="B17" s="101">
         <v>5.52</v>
       </c>
-      <c r="C17" s="110" t="s">
+      <c r="C17" s="95" t="s">
         <v>256</v>
       </c>
-      <c r="D17" s="110" t="s">
+      <c r="D17" s="95" t="s">
         <v>283</v>
       </c>
-      <c r="E17" s="110"/>
-      <c r="F17" s="111"/>
+      <c r="E17" s="95"/>
+      <c r="F17" s="96"/>
     </row>
     <row r="18" spans="1:6" ht="90">
-      <c r="A18" s="118" t="s">
+      <c r="A18" s="100" t="s">
         <v>242</v>
       </c>
-      <c r="B18" s="120">
+      <c r="B18" s="101">
         <v>7.89</v>
       </c>
-      <c r="C18" s="110" t="s">
+      <c r="C18" s="95" t="s">
         <v>282</v>
       </c>
-      <c r="D18" s="110" t="s">
+      <c r="D18" s="95" t="s">
         <v>284</v>
       </c>
-      <c r="E18" s="110" t="s">
+      <c r="E18" s="95" t="s">
         <v>285</v>
       </c>
-      <c r="F18" s="111"/>
+      <c r="F18" s="96"/>
     </row>
     <row r="19" spans="1:6">
-      <c r="A19" s="118" t="s">
+      <c r="A19" s="100" t="s">
         <v>243</v>
       </c>
-      <c r="B19" s="120">
+      <c r="B19" s="101">
         <v>3.2</v>
       </c>
-      <c r="C19" s="110" t="s">
+      <c r="C19" s="95" t="s">
         <v>256</v>
       </c>
-      <c r="D19" s="110" t="s">
+      <c r="D19" s="95" t="s">
         <v>268</v>
       </c>
-      <c r="E19" s="110"/>
-      <c r="F19" s="111"/>
+      <c r="E19" s="95"/>
+      <c r="F19" s="96"/>
     </row>
     <row r="20" spans="1:6" ht="45">
-      <c r="A20" s="118" t="s">
+      <c r="A20" s="100" t="s">
         <v>244</v>
       </c>
-      <c r="B20" s="120">
+      <c r="B20" s="101">
         <v>11.14</v>
       </c>
-      <c r="C20" s="110" t="s">
+      <c r="C20" s="95" t="s">
         <v>256</v>
       </c>
-      <c r="D20" s="110" t="s">
+      <c r="D20" s="95" t="s">
         <v>268</v>
       </c>
-      <c r="E20" s="110" t="s">
+      <c r="E20" s="95" t="s">
         <v>288</v>
       </c>
-      <c r="F20" s="111"/>
+      <c r="F20" s="96"/>
     </row>
     <row r="21" spans="1:6" ht="45">
-      <c r="A21" s="118" t="s">
+      <c r="A21" s="100" t="s">
         <v>245</v>
       </c>
-      <c r="B21" s="120">
+      <c r="B21" s="101">
         <v>11.59</v>
       </c>
-      <c r="C21" s="110" t="s">
+      <c r="C21" s="95" t="s">
         <v>256</v>
       </c>
-      <c r="D21" s="110" t="s">
+      <c r="D21" s="95" t="s">
         <v>268</v>
       </c>
-      <c r="E21" s="110" t="s">
+      <c r="E21" s="95" t="s">
         <v>288</v>
       </c>
-      <c r="F21" s="111"/>
+      <c r="F21" s="96"/>
     </row>
     <row r="22" spans="1:6" ht="30">
-      <c r="A22" s="118" t="s">
+      <c r="A22" s="100" t="s">
         <v>246</v>
       </c>
-      <c r="B22" s="120">
+      <c r="B22" s="101">
         <v>13.8</v>
       </c>
-      <c r="C22" s="110" t="s">
+      <c r="C22" s="95" t="s">
         <v>286</v>
       </c>
-      <c r="D22" s="110" t="s">
+      <c r="D22" s="95" t="s">
         <v>268</v>
       </c>
-      <c r="E22" s="110" t="s">
+      <c r="E22" s="95" t="s">
         <v>289</v>
       </c>
-      <c r="F22" s="109"/>
+      <c r="F22" s="94"/>
     </row>
     <row r="23" spans="1:6">
-      <c r="C23" s="108"/>
-      <c r="D23" s="108"/>
-      <c r="E23" s="108"/>
+      <c r="C23" s="93"/>
+      <c r="D23" s="93"/>
+      <c r="E23" s="93"/>
     </row>
     <row r="24" spans="1:6">
-      <c r="C24" s="108"/>
-      <c r="D24" s="108"/>
-      <c r="E24" s="108"/>
+      <c r="C24" s="93"/>
+      <c r="D24" s="93"/>
+      <c r="E24" s="93"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
elektryka w łazience i sumy
</commit_message>
<xml_diff>
--- a/plan/Mati - do uzgodnienia.xlsx
+++ b/plan/Mati - do uzgodnienia.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="2505" windowWidth="17010" windowHeight="5520" tabRatio="854" activeTab="6"/>
@@ -15,12 +15,12 @@
     <sheet name="Instalacje - uzgodnienia" sheetId="11" r:id="rId6"/>
     <sheet name="Gniazdka" sheetId="12" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="499" uniqueCount="331">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="498" uniqueCount="331">
   <si>
     <t>Piwnica</t>
   </si>
@@ -1433,7 +1433,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="134">
+  <cellXfs count="135">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1744,6 +1744,7 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1793,12 +1794,292 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="21">
+  <dxfs count="41">
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="none">
@@ -1978,33 +2259,69 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:T17" totalsRowShown="0" dataDxfId="3">
-  <autoFilter ref="A1:T17">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:T18" totalsRowCount="1" dataDxfId="40">
+  <autoFilter ref="A1:T18">
     <filterColumn colId="1"/>
     <filterColumn colId="6"/>
     <filterColumn colId="10"/>
   </autoFilter>
   <tableColumns count="20">
-    <tableColumn id="1" name="Kolumna1" dataDxfId="20"/>
-    <tableColumn id="20" name="Kolumna2" dataDxfId="0"/>
-    <tableColumn id="2" name="Włącznik 1" dataDxfId="19"/>
-    <tableColumn id="3" name="Włącznik 2" dataDxfId="18"/>
-    <tableColumn id="4" name="W krzyżowy" dataDxfId="17"/>
-    <tableColumn id="5" name="W schodowy 1" dataDxfId="16"/>
-    <tableColumn id="18" name="W schodowy 2" dataDxfId="2"/>
-    <tableColumn id="6" name="Gniazdko 1" dataDxfId="15"/>
-    <tableColumn id="7" name="Gniazdko 2" dataDxfId="14"/>
-    <tableColumn id="8" name="Gniazdko H" dataDxfId="13"/>
-    <tableColumn id="19" name="Natynkowe" dataDxfId="1"/>
-    <tableColumn id="9" name="Głośnik 1" dataDxfId="12"/>
-    <tableColumn id="10" name="Głośnik 2" dataDxfId="11"/>
-    <tableColumn id="11" name="Sat" dataDxfId="10"/>
-    <tableColumn id="12" name="komp" dataDxfId="9"/>
-    <tableColumn id="13" name="Ramka1" dataDxfId="8"/>
-    <tableColumn id="14" name="Ramka2" dataDxfId="7"/>
-    <tableColumn id="15" name="Ramka3" dataDxfId="6"/>
-    <tableColumn id="16" name="Ramka4" dataDxfId="5"/>
-    <tableColumn id="17" name="Ramka5" dataDxfId="4"/>
+    <tableColumn id="1" name="Kolumna1" dataDxfId="39" totalsRowDxfId="19"/>
+    <tableColumn id="20" name="Kolumna2" dataDxfId="38" totalsRowDxfId="18"/>
+    <tableColumn id="2" name="Włącznik 1" totalsRowFunction="custom" dataDxfId="37" totalsRowDxfId="17">
+      <totalsRowFormula>SUM([Włącznik 1])</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="3" name="Włącznik 2" totalsRowFunction="custom" dataDxfId="36" totalsRowDxfId="16">
+      <totalsRowFormula>SUM([Włącznik 2])</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="4" name="W krzyżowy" totalsRowFunction="custom" dataDxfId="35" totalsRowDxfId="15">
+      <totalsRowFormula>SUM([W krzyżowy])</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="5" name="W schodowy 1" totalsRowFunction="custom" dataDxfId="34" totalsRowDxfId="14">
+      <totalsRowFormula>SUM([W schodowy 1])</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="18" name="W schodowy 2" totalsRowFunction="custom" dataDxfId="33" totalsRowDxfId="13">
+      <totalsRowFormula>SUM([W schodowy 2])</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="6" name="Gniazdko 1" totalsRowFunction="custom" dataDxfId="32" totalsRowDxfId="12">
+      <totalsRowFormula>SUM([Gniazdko 1])</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="7" name="Gniazdko 2" totalsRowFunction="custom" dataDxfId="31" totalsRowDxfId="11">
+      <totalsRowFormula>SUM([Gniazdko 2])</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="8" name="Gniazdko H" totalsRowFunction="custom" dataDxfId="30" totalsRowDxfId="10">
+      <totalsRowFormula>SUM([Gniazdko H])</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="19" name="Natynkowe" totalsRowFunction="custom" dataDxfId="29" totalsRowDxfId="9">
+      <totalsRowFormula>SUM([Natynkowe])</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="9" name="Głośnik 1" totalsRowFunction="custom" dataDxfId="28" totalsRowDxfId="8">
+      <totalsRowFormula>SUM([Głośnik 1])</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="10" name="Głośnik 2" totalsRowFunction="custom" dataDxfId="27" totalsRowDxfId="7">
+      <totalsRowFormula>SUM([Głośnik 2])</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="11" name="Sat" totalsRowFunction="custom" dataDxfId="26" totalsRowDxfId="6">
+      <totalsRowFormula>SUM([Sat])</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="12" name="komp" totalsRowFunction="custom" dataDxfId="25" totalsRowDxfId="5">
+      <totalsRowFormula>SUM([komp])</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="13" name="Ramka1" totalsRowFunction="custom" dataDxfId="24" totalsRowDxfId="4">
+      <totalsRowFormula>SUM([Ramka1])</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="14" name="Ramka2" totalsRowFunction="custom" dataDxfId="23" totalsRowDxfId="3">
+      <totalsRowFormula>SUM([Ramka2])</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="15" name="Ramka3" totalsRowFunction="custom" dataDxfId="22" totalsRowDxfId="2">
+      <totalsRowFormula>SUM([Ramka3])</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="16" name="Ramka4" totalsRowFunction="custom" dataDxfId="21" totalsRowDxfId="1">
+      <totalsRowFormula>SUM([Ramka4])</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="17" name="Ramka5" totalsRowFunction="custom" dataDxfId="20" totalsRowDxfId="0">
+      <totalsRowFormula>SUM([Ramka5])</totalsRowFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium19" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2351,7 +2668,7 @@
       <c r="L1" s="4"/>
     </row>
     <row r="2" spans="1:12" ht="52.5">
-      <c r="A2" s="114" t="s">
+      <c r="A2" s="115" t="s">
         <v>25</v>
       </c>
       <c r="B2" s="61" t="s">
@@ -2379,7 +2696,7 @@
       </c>
     </row>
     <row r="3" spans="1:12" ht="126">
-      <c r="A3" s="114"/>
+      <c r="A3" s="115"/>
       <c r="B3" s="61" t="s">
         <v>26</v>
       </c>
@@ -2413,7 +2730,7 @@
       <c r="J4" s="65"/>
     </row>
     <row r="5" spans="1:12" ht="31.5">
-      <c r="A5" s="115" t="s">
+      <c r="A5" s="116" t="s">
         <v>24</v>
       </c>
       <c r="B5" s="61" t="s">
@@ -2431,7 +2748,7 @@
       <c r="J5" s="65"/>
     </row>
     <row r="6" spans="1:12" ht="21">
-      <c r="A6" s="114"/>
+      <c r="A6" s="115"/>
       <c r="B6" s="61" t="s">
         <v>9</v>
       </c>
@@ -2451,7 +2768,7 @@
       <c r="J6" s="65"/>
     </row>
     <row r="7" spans="1:12" ht="21">
-      <c r="A7" s="114"/>
+      <c r="A7" s="115"/>
       <c r="B7" s="61" t="s">
         <v>10</v>
       </c>
@@ -2471,7 +2788,7 @@
       <c r="J7" s="65"/>
     </row>
     <row r="8" spans="1:12" ht="21">
-      <c r="A8" s="114"/>
+      <c r="A8" s="115"/>
       <c r="B8" s="61" t="s">
         <v>12</v>
       </c>
@@ -2491,7 +2808,7 @@
       <c r="J8" s="65"/>
     </row>
     <row r="9" spans="1:12" ht="21">
-      <c r="A9" s="116"/>
+      <c r="A9" s="117"/>
       <c r="B9" s="61" t="s">
         <v>8</v>
       </c>
@@ -2858,7 +3175,7 @@
       </c>
     </row>
     <row r="2" spans="1:12" ht="15">
-      <c r="A2" s="117" t="s">
+      <c r="A2" s="118" t="s">
         <v>106</v>
       </c>
       <c r="B2" s="32" t="s">
@@ -2879,7 +3196,7 @@
       </c>
     </row>
     <row r="3" spans="1:12" ht="85.5">
-      <c r="A3" s="118"/>
+      <c r="A3" s="119"/>
       <c r="B3" s="45" t="s">
         <v>55</v>
       </c>
@@ -2898,7 +3215,7 @@
       <c r="L3"/>
     </row>
     <row r="4" spans="1:12" ht="17.25" customHeight="1" thickBot="1">
-      <c r="A4" s="119"/>
+      <c r="A4" s="120"/>
       <c r="B4" s="44" t="s">
         <v>96</v>
       </c>
@@ -2917,7 +3234,7 @@
       </c>
     </row>
     <row r="5" spans="1:12" ht="15">
-      <c r="A5" s="120" t="s">
+      <c r="A5" s="121" t="s">
         <v>98</v>
       </c>
       <c r="B5" s="80" t="s">
@@ -2944,7 +3261,7 @@
       </c>
     </row>
     <row r="6" spans="1:12" ht="33">
-      <c r="A6" s="121"/>
+      <c r="A6" s="122"/>
       <c r="B6" s="42" t="s">
         <v>133</v>
       </c>
@@ -2963,7 +3280,7 @@
       <c r="L6"/>
     </row>
     <row r="7" spans="1:12" ht="22.5">
-      <c r="A7" s="121"/>
+      <c r="A7" s="122"/>
       <c r="B7" s="38" t="s">
         <v>72</v>
       </c>
@@ -2990,7 +3307,7 @@
       </c>
     </row>
     <row r="8" spans="1:12" ht="54">
-      <c r="A8" s="121"/>
+      <c r="A8" s="122"/>
       <c r="B8" s="85" t="s">
         <v>73</v>
       </c>
@@ -3013,7 +3330,7 @@
       </c>
     </row>
     <row r="9" spans="1:12" ht="52.5">
-      <c r="A9" s="121"/>
+      <c r="A9" s="122"/>
       <c r="B9" s="85" t="s">
         <v>90</v>
       </c>
@@ -3031,7 +3348,7 @@
       </c>
     </row>
     <row r="10" spans="1:12" ht="21">
-      <c r="A10" s="121"/>
+      <c r="A10" s="122"/>
       <c r="B10" s="85" t="s">
         <v>75</v>
       </c>
@@ -3049,8 +3366,8 @@
       </c>
     </row>
     <row r="11" spans="1:12" ht="31.5">
-      <c r="A11" s="121"/>
-      <c r="B11" s="122" t="s">
+      <c r="A11" s="122"/>
+      <c r="B11" s="123" t="s">
         <v>136</v>
       </c>
       <c r="C11" s="86" t="s">
@@ -3067,8 +3384,8 @@
       </c>
     </row>
     <row r="12" spans="1:12" ht="21">
-      <c r="A12" s="121"/>
-      <c r="B12" s="124"/>
+      <c r="A12" s="122"/>
+      <c r="B12" s="125"/>
       <c r="C12" s="86" t="s">
         <v>141</v>
       </c>
@@ -3083,8 +3400,8 @@
       </c>
     </row>
     <row r="13" spans="1:12" ht="31.5">
-      <c r="A13" s="121"/>
-      <c r="B13" s="123"/>
+      <c r="A13" s="122"/>
+      <c r="B13" s="124"/>
       <c r="C13" s="17" t="s">
         <v>142</v>
       </c>
@@ -3097,7 +3414,7 @@
       <c r="J13" s="19"/>
     </row>
     <row r="14" spans="1:12">
-      <c r="A14" s="121"/>
+      <c r="A14" s="122"/>
       <c r="B14" s="38" t="s">
         <v>83</v>
       </c>
@@ -3113,8 +3430,8 @@
       <c r="J14" s="55"/>
     </row>
     <row r="15" spans="1:12" ht="42">
-      <c r="A15" s="121"/>
-      <c r="B15" s="122" t="s">
+      <c r="A15" s="122"/>
+      <c r="B15" s="123" t="s">
         <v>138</v>
       </c>
       <c r="C15" s="17" t="s">
@@ -3129,8 +3446,8 @@
       <c r="J15" s="19"/>
     </row>
     <row r="16" spans="1:12" ht="21">
-      <c r="A16" s="121"/>
-      <c r="B16" s="123"/>
+      <c r="A16" s="122"/>
+      <c r="B16" s="124"/>
       <c r="C16" s="9" t="s">
         <v>169</v>
       </c>
@@ -3147,7 +3464,7 @@
       <c r="J16" s="56"/>
     </row>
     <row r="17" spans="1:11" ht="31.5">
-      <c r="A17" s="121"/>
+      <c r="A17" s="122"/>
       <c r="B17" s="43" t="s">
         <v>96</v>
       </c>
@@ -3173,7 +3490,7 @@
       <c r="J17" s="57"/>
     </row>
     <row r="18" spans="1:11">
-      <c r="A18" s="121"/>
+      <c r="A18" s="122"/>
       <c r="B18" s="43" t="s">
         <v>99</v>
       </c>
@@ -3189,7 +3506,7 @@
       <c r="J18" s="21"/>
     </row>
     <row r="19" spans="1:11">
-      <c r="A19" s="121"/>
+      <c r="A19" s="122"/>
       <c r="B19" s="43" t="s">
         <v>104</v>
       </c>
@@ -3207,7 +3524,7 @@
       <c r="J19" s="21"/>
     </row>
     <row r="20" spans="1:11" ht="31.5">
-      <c r="A20" s="121"/>
+      <c r="A20" s="122"/>
       <c r="B20" s="43" t="s">
         <v>102</v>
       </c>
@@ -3223,7 +3540,7 @@
       <c r="J20" s="11"/>
     </row>
     <row r="21" spans="1:11" ht="21">
-      <c r="A21" s="121"/>
+      <c r="A21" s="122"/>
       <c r="B21" s="92" t="s">
         <v>29</v>
       </c>
@@ -3241,7 +3558,7 @@
       </c>
     </row>
     <row r="22" spans="1:11" ht="42.75" thickBot="1">
-      <c r="A22" s="119"/>
+      <c r="A22" s="120"/>
       <c r="B22" s="44" t="s">
         <v>103</v>
       </c>
@@ -3261,7 +3578,7 @@
       <c r="J22" s="14"/>
     </row>
     <row r="23" spans="1:11">
-      <c r="A23" s="120" t="s">
+      <c r="A23" s="121" t="s">
         <v>63</v>
       </c>
       <c r="B23" s="80" t="s">
@@ -3281,7 +3598,7 @@
       </c>
     </row>
     <row r="24" spans="1:11" ht="31.5">
-      <c r="A24" s="121"/>
+      <c r="A24" s="122"/>
       <c r="B24" s="98" t="s">
         <v>67</v>
       </c>
@@ -3303,7 +3620,7 @@
       </c>
     </row>
     <row r="25" spans="1:11" ht="63">
-      <c r="A25" s="121"/>
+      <c r="A25" s="122"/>
       <c r="B25" s="43" t="s">
         <v>100</v>
       </c>
@@ -3321,7 +3638,7 @@
       <c r="J25" s="21"/>
     </row>
     <row r="26" spans="1:11" ht="11.25" thickBot="1">
-      <c r="A26" s="119"/>
+      <c r="A26" s="120"/>
       <c r="B26" s="44" t="s">
         <v>96</v>
       </c>
@@ -3834,10 +4151,10 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="31.5">
-      <c r="A2" s="125" t="s">
+      <c r="A2" s="126" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="126" t="s">
+      <c r="B2" s="127" t="s">
         <v>95</v>
       </c>
       <c r="C2" s="23" t="s">
@@ -3856,8 +4173,8 @@
       <c r="J2" s="23"/>
     </row>
     <row r="3" spans="1:10" ht="31.5">
-      <c r="A3" s="125"/>
-      <c r="B3" s="126"/>
+      <c r="A3" s="126"/>
+      <c r="B3" s="127"/>
       <c r="C3" s="101" t="s">
         <v>130</v>
       </c>
@@ -3878,7 +4195,7 @@
       </c>
     </row>
     <row r="4" spans="1:10" ht="31.5">
-      <c r="A4" s="125" t="s">
+      <c r="A4" s="126" t="s">
         <v>154</v>
       </c>
       <c r="B4" s="36" t="s">
@@ -3898,7 +4215,7 @@
       <c r="J4" s="23"/>
     </row>
     <row r="5" spans="1:10">
-      <c r="A5" s="125"/>
+      <c r="A5" s="126"/>
       <c r="B5" s="103" t="s">
         <v>156</v>
       </c>
@@ -3918,8 +4235,8 @@
       <c r="J5" s="101"/>
     </row>
     <row r="6" spans="1:10" ht="73.5">
-      <c r="A6" s="125"/>
-      <c r="B6" s="126" t="s">
+      <c r="A6" s="126"/>
+      <c r="B6" s="127" t="s">
         <v>33</v>
       </c>
       <c r="C6" s="26" t="s">
@@ -3942,8 +4259,8 @@
       <c r="J6" s="26"/>
     </row>
     <row r="7" spans="1:10" ht="42">
-      <c r="A7" s="125"/>
-      <c r="B7" s="126"/>
+      <c r="A7" s="126"/>
+      <c r="B7" s="127"/>
       <c r="C7" s="104" t="s">
         <v>87</v>
       </c>
@@ -3962,8 +4279,8 @@
       </c>
     </row>
     <row r="8" spans="1:10" ht="42.75" thickBot="1">
-      <c r="A8" s="125"/>
-      <c r="B8" s="127" t="s">
+      <c r="A8" s="126"/>
+      <c r="B8" s="128" t="s">
         <v>29</v>
       </c>
       <c r="C8" s="2" t="s">
@@ -3986,8 +4303,8 @@
       <c r="J8" s="2"/>
     </row>
     <row r="9" spans="1:10" ht="31.5">
-      <c r="A9" s="125"/>
-      <c r="B9" s="127"/>
+      <c r="A9" s="126"/>
+      <c r="B9" s="128"/>
       <c r="C9" s="105" t="s">
         <v>32</v>
       </c>
@@ -4004,7 +4321,7 @@
       </c>
     </row>
     <row r="10" spans="1:10" ht="52.5">
-      <c r="A10" s="125" t="s">
+      <c r="A10" s="126" t="s">
         <v>157</v>
       </c>
       <c r="B10" s="36" t="s">
@@ -4022,7 +4339,7 @@
       <c r="J10" s="26"/>
     </row>
     <row r="11" spans="1:10" ht="52.5">
-      <c r="A11" s="125"/>
+      <c r="A11" s="126"/>
       <c r="B11" s="109" t="s">
         <v>166</v>
       </c>
@@ -4048,7 +4365,7 @@
       </c>
     </row>
     <row r="12" spans="1:10" ht="41.25" customHeight="1">
-      <c r="A12" s="125"/>
+      <c r="A12" s="126"/>
       <c r="B12" s="109" t="s">
         <v>165</v>
       </c>
@@ -4223,7 +4540,7 @@
       </c>
     </row>
     <row r="3" spans="1:10" ht="52.5">
-      <c r="A3" s="128" t="s">
+      <c r="A3" s="129" t="s">
         <v>173</v>
       </c>
       <c r="B3" s="111" t="s">
@@ -4245,7 +4562,7 @@
       </c>
     </row>
     <row r="4" spans="1:10" ht="31.5">
-      <c r="A4" s="128"/>
+      <c r="A4" s="129"/>
       <c r="B4" s="111" t="s">
         <v>177</v>
       </c>
@@ -4267,7 +4584,7 @@
       </c>
     </row>
     <row r="5" spans="1:10" ht="21">
-      <c r="A5" s="128"/>
+      <c r="A5" s="129"/>
       <c r="B5" s="111" t="s">
         <v>219</v>
       </c>
@@ -4287,7 +4604,7 @@
       </c>
     </row>
     <row r="6" spans="1:10" ht="52.5">
-      <c r="A6" s="128"/>
+      <c r="A6" s="129"/>
       <c r="B6" s="111" t="s">
         <v>178</v>
       </c>
@@ -4606,14 +4923,14 @@
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" thickBot="1"/>
     <row r="2" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A2" s="129" t="s">
+      <c r="A2" s="130" t="s">
         <v>249</v>
       </c>
-      <c r="B2" s="130"/>
-      <c r="C2" s="131"/>
-      <c r="D2" s="131"/>
-      <c r="E2" s="131"/>
-      <c r="F2" s="132"/>
+      <c r="B2" s="131"/>
+      <c r="C2" s="132"/>
+      <c r="D2" s="132"/>
+      <c r="E2" s="132"/>
+      <c r="F2" s="133"/>
     </row>
     <row r="3" spans="1:6" ht="30">
       <c r="A3" s="76" t="s">
@@ -4987,7 +5304,7 @@
   <dimension ref="A1:T39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5004,8 +5321,8 @@
     <col min="11" max="11" width="7.28515625" customWidth="1"/>
     <col min="12" max="12" width="6.42578125" customWidth="1"/>
     <col min="13" max="13" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.28515625" style="133" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.85546875" style="133" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.28515625" style="114" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.85546875" style="114" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="9.85546875" customWidth="1"/>
     <col min="17" max="17" width="7.85546875" customWidth="1"/>
     <col min="18" max="18" width="7.42578125" customWidth="1"/>
@@ -5054,10 +5371,10 @@
       <c r="M1" t="s">
         <v>306</v>
       </c>
-      <c r="N1" s="133" t="s">
+      <c r="N1" s="114" t="s">
         <v>312</v>
       </c>
-      <c r="O1" s="133" t="s">
+      <c r="O1" s="114" t="s">
         <v>313</v>
       </c>
       <c r="P1" t="s">
@@ -5077,521 +5394,579 @@
       </c>
     </row>
     <row r="2" spans="1:20">
-      <c r="A2" s="133" t="s">
+      <c r="A2" s="114" t="s">
         <v>300</v>
       </c>
-      <c r="B2" s="133"/>
-      <c r="C2" s="133">
-        <v>1</v>
-      </c>
-      <c r="D2" s="133"/>
-      <c r="E2" s="133"/>
-      <c r="F2" s="133">
-        <v>1</v>
-      </c>
-      <c r="G2" s="133"/>
-      <c r="H2" s="133"/>
-      <c r="I2" s="133">
-        <v>1</v>
-      </c>
-      <c r="J2" s="133"/>
-      <c r="K2" s="133"/>
-      <c r="L2" s="133"/>
-      <c r="M2" s="133"/>
-      <c r="P2" s="133">
-        <v>1</v>
-      </c>
-      <c r="Q2" s="133">
-        <v>1</v>
-      </c>
-      <c r="R2" s="133"/>
-      <c r="S2" s="133"/>
+      <c r="B2" s="114"/>
+      <c r="C2" s="114">
+        <v>1</v>
+      </c>
+      <c r="D2" s="114"/>
+      <c r="E2" s="114"/>
+      <c r="F2" s="114">
+        <v>1</v>
+      </c>
+      <c r="G2" s="114"/>
+      <c r="H2" s="114"/>
+      <c r="I2" s="114">
+        <v>1</v>
+      </c>
+      <c r="J2" s="114"/>
+      <c r="K2" s="114"/>
+      <c r="L2" s="114"/>
+      <c r="M2" s="114"/>
+      <c r="P2" s="114">
+        <v>1</v>
+      </c>
+      <c r="Q2" s="114">
+        <v>1</v>
+      </c>
+      <c r="R2" s="114"/>
+      <c r="S2" s="114"/>
     </row>
     <row r="3" spans="1:20">
-      <c r="A3" s="133" t="s">
+      <c r="A3" s="114" t="s">
         <v>173</v>
       </c>
-      <c r="B3" s="133"/>
-      <c r="C3" s="133">
+      <c r="B3" s="114"/>
+      <c r="C3" s="114">
         <v>2</v>
       </c>
-      <c r="D3" s="133"/>
-      <c r="E3" s="133"/>
-      <c r="F3" s="133"/>
-      <c r="G3" s="133"/>
-      <c r="H3" s="133">
+      <c r="D3" s="114"/>
+      <c r="E3" s="114"/>
+      <c r="F3" s="114"/>
+      <c r="G3" s="114"/>
+      <c r="H3" s="114">
         <v>5</v>
       </c>
-      <c r="I3" s="133">
+      <c r="I3" s="114">
         <v>3</v>
       </c>
-      <c r="J3" s="133"/>
-      <c r="K3" s="133"/>
-      <c r="L3" s="133"/>
-      <c r="M3" s="133"/>
-      <c r="P3" s="133">
+      <c r="J3" s="114"/>
+      <c r="K3" s="114"/>
+      <c r="L3" s="114"/>
+      <c r="M3" s="114"/>
+      <c r="P3" s="114">
         <v>2</v>
       </c>
-      <c r="Q3" s="133">
-        <v>1</v>
-      </c>
-      <c r="R3" s="133">
+      <c r="Q3" s="114">
+        <v>1</v>
+      </c>
+      <c r="R3" s="114">
         <v>2</v>
       </c>
-      <c r="S3" s="133"/>
+      <c r="S3" s="114"/>
     </row>
     <row r="4" spans="1:20">
-      <c r="A4" s="133" t="s">
+      <c r="A4" s="114" t="s">
         <v>189</v>
       </c>
-      <c r="B4" s="133"/>
-      <c r="C4" s="133"/>
-      <c r="D4" s="133"/>
-      <c r="E4" s="133"/>
-      <c r="F4" s="133"/>
-      <c r="G4" s="133"/>
-      <c r="H4" s="133"/>
-      <c r="I4" s="133">
+      <c r="B4" s="114"/>
+      <c r="C4" s="114"/>
+      <c r="D4" s="114"/>
+      <c r="E4" s="114"/>
+      <c r="F4" s="114"/>
+      <c r="G4" s="114"/>
+      <c r="H4" s="114"/>
+      <c r="I4" s="114">
         <v>2</v>
       </c>
-      <c r="J4" s="133"/>
-      <c r="K4" s="133"/>
-      <c r="L4" s="133"/>
-      <c r="M4" s="133"/>
-      <c r="P4" s="133">
+      <c r="J4" s="114"/>
+      <c r="K4" s="114"/>
+      <c r="L4" s="114"/>
+      <c r="M4" s="114"/>
+      <c r="P4" s="114">
         <v>2</v>
       </c>
-      <c r="Q4" s="133"/>
-      <c r="R4" s="133"/>
-      <c r="S4" s="133"/>
+      <c r="Q4" s="114"/>
+      <c r="R4" s="114"/>
+      <c r="S4" s="114"/>
     </row>
     <row r="5" spans="1:20">
-      <c r="A5" s="133" t="s">
+      <c r="A5" s="114" t="s">
         <v>172</v>
       </c>
-      <c r="B5" s="133"/>
-      <c r="C5" s="133">
-        <v>1</v>
-      </c>
-      <c r="D5" s="133">
+      <c r="B5" s="114"/>
+      <c r="C5" s="114">
+        <v>1</v>
+      </c>
+      <c r="D5" s="114">
         <v>2</v>
       </c>
-      <c r="E5" s="133">
-        <v>1</v>
-      </c>
-      <c r="F5" s="133"/>
-      <c r="G5" s="133"/>
-      <c r="H5" s="133">
-        <v>1</v>
-      </c>
-      <c r="I5" s="133">
+      <c r="E5" s="114">
+        <v>1</v>
+      </c>
+      <c r="F5" s="114"/>
+      <c r="G5" s="114"/>
+      <c r="H5" s="114">
+        <v>1</v>
+      </c>
+      <c r="I5" s="114">
         <v>5</v>
       </c>
-      <c r="J5" s="133"/>
-      <c r="K5" s="133"/>
-      <c r="L5" s="133">
+      <c r="J5" s="114"/>
+      <c r="K5" s="114"/>
+      <c r="L5" s="114">
         <v>4</v>
       </c>
-      <c r="M5" s="133">
+      <c r="M5" s="114">
         <v>2</v>
       </c>
-      <c r="N5" s="133">
+      <c r="N5" s="114">
         <v>2</v>
       </c>
-      <c r="O5" s="133">
-        <v>1</v>
-      </c>
-      <c r="P5" s="133">
-        <v>1</v>
-      </c>
-      <c r="Q5" s="133">
+      <c r="O5" s="114">
+        <v>1</v>
+      </c>
+      <c r="P5" s="114">
+        <v>1</v>
+      </c>
+      <c r="Q5" s="114">
         <v>5</v>
       </c>
-      <c r="R5" s="133">
-        <v>1</v>
-      </c>
-      <c r="S5" s="133"/>
-      <c r="T5" s="133">
+      <c r="R5" s="114">
+        <v>1</v>
+      </c>
+      <c r="S5" s="114"/>
+      <c r="T5" s="114">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:20">
-      <c r="A6" s="133" t="s">
+      <c r="A6" s="114" t="s">
         <v>315</v>
       </c>
-      <c r="B6" s="133"/>
-      <c r="C6" s="133">
+      <c r="B6" s="114"/>
+      <c r="C6" s="114">
         <v>2</v>
       </c>
-      <c r="D6" s="133">
-        <v>1</v>
-      </c>
-      <c r="E6" s="133"/>
-      <c r="F6" s="133">
+      <c r="D6" s="114">
+        <v>1</v>
+      </c>
+      <c r="E6" s="114"/>
+      <c r="F6" s="114">
         <v>3</v>
       </c>
-      <c r="G6" s="133"/>
-      <c r="H6" s="133">
-        <v>1</v>
-      </c>
-      <c r="I6" s="133">
-        <v>1</v>
-      </c>
-      <c r="J6" s="133"/>
-      <c r="K6" s="133"/>
-      <c r="L6" s="133"/>
-      <c r="M6" s="133"/>
-      <c r="P6" s="133">
+      <c r="G6" s="114"/>
+      <c r="H6" s="114">
+        <v>1</v>
+      </c>
+      <c r="I6" s="114">
+        <v>1</v>
+      </c>
+      <c r="J6" s="114"/>
+      <c r="K6" s="114"/>
+      <c r="L6" s="114"/>
+      <c r="M6" s="114"/>
+      <c r="P6" s="114">
         <v>4</v>
       </c>
-      <c r="Q6" s="133">
+      <c r="Q6" s="114">
         <v>2</v>
       </c>
-      <c r="R6" s="133"/>
-      <c r="S6" s="133"/>
-      <c r="T6" s="133"/>
+      <c r="R6" s="114"/>
+      <c r="S6" s="114"/>
+      <c r="T6" s="114"/>
     </row>
     <row r="7" spans="1:20">
-      <c r="A7" s="133" t="s">
+      <c r="A7" s="114" t="s">
         <v>316</v>
       </c>
-      <c r="B7" s="133"/>
-      <c r="C7" s="133" t="s">
-        <v>317</v>
-      </c>
-      <c r="D7" s="133"/>
-      <c r="E7" s="133"/>
-      <c r="F7" s="133"/>
-      <c r="G7" s="133"/>
-      <c r="H7" s="133"/>
-      <c r="I7" s="133"/>
-      <c r="J7" s="133"/>
-      <c r="K7" s="133"/>
-      <c r="L7" s="133"/>
-      <c r="M7" s="133"/>
-      <c r="P7" s="133"/>
-      <c r="Q7" s="133"/>
-      <c r="R7" s="133"/>
-      <c r="S7" s="133"/>
-      <c r="T7" s="133"/>
+      <c r="B7" s="114"/>
+      <c r="C7" s="114">
+        <v>1</v>
+      </c>
+      <c r="D7" s="114"/>
+      <c r="E7" s="114"/>
+      <c r="F7" s="114"/>
+      <c r="G7" s="114"/>
+      <c r="H7" s="114"/>
+      <c r="I7" s="114"/>
+      <c r="J7" s="114">
+        <v>2</v>
+      </c>
+      <c r="K7" s="114"/>
+      <c r="L7" s="114"/>
+      <c r="M7" s="114"/>
+      <c r="P7" s="114"/>
+      <c r="Q7" s="114"/>
+      <c r="R7" s="114"/>
+      <c r="S7" s="114"/>
+      <c r="T7" s="114"/>
     </row>
     <row r="8" spans="1:20">
-      <c r="A8" s="133" t="s">
+      <c r="A8" s="114" t="s">
         <v>318</v>
       </c>
-      <c r="B8" s="133"/>
-      <c r="C8" s="133"/>
-      <c r="D8" s="133"/>
-      <c r="E8" s="133"/>
-      <c r="F8" s="133"/>
-      <c r="G8" s="133"/>
-      <c r="H8" s="133"/>
-      <c r="I8" s="133"/>
-      <c r="J8" s="133">
+      <c r="B8" s="114"/>
+      <c r="C8" s="114"/>
+      <c r="D8" s="114"/>
+      <c r="E8" s="114"/>
+      <c r="F8" s="114"/>
+      <c r="G8" s="114"/>
+      <c r="H8" s="114"/>
+      <c r="I8" s="114"/>
+      <c r="J8" s="114">
         <v>5</v>
       </c>
-      <c r="K8" s="133"/>
-      <c r="L8" s="133"/>
-      <c r="M8" s="133"/>
-      <c r="P8" s="133">
+      <c r="K8" s="114"/>
+      <c r="L8" s="114"/>
+      <c r="M8" s="114"/>
+      <c r="P8" s="114">
         <v>5</v>
       </c>
-      <c r="Q8" s="133"/>
-      <c r="R8" s="133"/>
-      <c r="S8" s="133"/>
-      <c r="T8" s="133"/>
+      <c r="Q8" s="114"/>
+      <c r="R8" s="114"/>
+      <c r="S8" s="114"/>
+      <c r="T8" s="114"/>
     </row>
     <row r="9" spans="1:20">
-      <c r="A9" s="133" t="s">
+      <c r="A9" s="114" t="s">
         <v>321</v>
       </c>
-      <c r="B9" s="133"/>
-      <c r="C9" s="133"/>
-      <c r="D9" s="133"/>
-      <c r="E9" s="133">
-        <v>1</v>
-      </c>
-      <c r="F9" s="133"/>
-      <c r="G9" s="133">
-        <v>1</v>
-      </c>
-      <c r="H9" s="133"/>
-      <c r="I9" s="133"/>
-      <c r="J9" s="133"/>
-      <c r="K9" s="133"/>
-      <c r="L9" s="133"/>
-      <c r="M9" s="133"/>
-      <c r="P9" s="133"/>
-      <c r="Q9" s="133">
-        <v>1</v>
-      </c>
-      <c r="R9" s="133"/>
-      <c r="S9" s="133"/>
-      <c r="T9" s="133"/>
+      <c r="B9" s="114"/>
+      <c r="C9" s="114"/>
+      <c r="D9" s="114"/>
+      <c r="E9" s="114">
+        <v>1</v>
+      </c>
+      <c r="F9" s="114"/>
+      <c r="G9" s="114">
+        <v>1</v>
+      </c>
+      <c r="H9" s="114"/>
+      <c r="I9" s="114"/>
+      <c r="J9" s="114"/>
+      <c r="K9" s="114"/>
+      <c r="L9" s="114"/>
+      <c r="M9" s="114"/>
+      <c r="P9" s="114"/>
+      <c r="Q9" s="114">
+        <v>1</v>
+      </c>
+      <c r="R9" s="114"/>
+      <c r="S9" s="114"/>
+      <c r="T9" s="114"/>
     </row>
     <row r="10" spans="1:20">
-      <c r="A10" s="133" t="s">
+      <c r="A10" s="114" t="s">
         <v>323</v>
       </c>
-      <c r="B10" s="133"/>
-      <c r="C10" s="133">
+      <c r="B10" s="114"/>
+      <c r="C10" s="114">
         <v>2</v>
       </c>
-      <c r="D10" s="133"/>
-      <c r="E10" s="133"/>
-      <c r="F10" s="133"/>
-      <c r="G10" s="133"/>
-      <c r="H10" s="133"/>
-      <c r="I10" s="133"/>
-      <c r="J10" s="133">
+      <c r="D10" s="114"/>
+      <c r="E10" s="114"/>
+      <c r="F10" s="114"/>
+      <c r="G10" s="114"/>
+      <c r="H10" s="114"/>
+      <c r="I10" s="114"/>
+      <c r="J10" s="114">
         <v>3</v>
       </c>
-      <c r="K10" s="133"/>
-      <c r="L10" s="133"/>
-      <c r="M10" s="133"/>
-      <c r="P10" s="133">
-        <v>1</v>
-      </c>
-      <c r="Q10" s="133">
+      <c r="K10" s="114"/>
+      <c r="L10" s="114"/>
+      <c r="M10" s="114"/>
+      <c r="P10" s="114">
+        <v>1</v>
+      </c>
+      <c r="Q10" s="114">
         <v>2</v>
       </c>
-      <c r="R10" s="133"/>
-      <c r="S10" s="133"/>
-      <c r="T10" s="133"/>
+      <c r="R10" s="114"/>
+      <c r="S10" s="114"/>
+      <c r="T10" s="114"/>
     </row>
     <row r="11" spans="1:20">
-      <c r="A11" s="133" t="s">
+      <c r="A11" s="114" t="s">
         <v>324</v>
       </c>
-      <c r="B11" s="133"/>
-      <c r="C11" s="133">
+      <c r="B11" s="114"/>
+      <c r="C11" s="114">
         <v>2</v>
       </c>
-      <c r="D11" s="133"/>
-      <c r="E11" s="133"/>
-      <c r="F11" s="133">
+      <c r="D11" s="114"/>
+      <c r="E11" s="114"/>
+      <c r="F11" s="114">
         <v>2</v>
       </c>
-      <c r="G11" s="133">
-        <v>1</v>
-      </c>
-      <c r="H11" s="133"/>
-      <c r="I11" s="133">
-        <v>1</v>
-      </c>
-      <c r="J11" s="133"/>
-      <c r="K11" s="133"/>
-      <c r="L11" s="133"/>
-      <c r="M11" s="133"/>
-      <c r="P11" s="133">
-        <v>1</v>
-      </c>
-      <c r="Q11" s="133">
-        <v>1</v>
-      </c>
-      <c r="R11" s="133">
-        <v>1</v>
-      </c>
-      <c r="S11" s="133"/>
-      <c r="T11" s="133"/>
+      <c r="G11" s="114">
+        <v>1</v>
+      </c>
+      <c r="H11" s="114"/>
+      <c r="I11" s="114">
+        <v>1</v>
+      </c>
+      <c r="J11" s="114"/>
+      <c r="K11" s="114"/>
+      <c r="L11" s="114"/>
+      <c r="M11" s="114"/>
+      <c r="P11" s="114">
+        <v>1</v>
+      </c>
+      <c r="Q11" s="114">
+        <v>1</v>
+      </c>
+      <c r="R11" s="114">
+        <v>1</v>
+      </c>
+      <c r="S11" s="114"/>
+      <c r="T11" s="114"/>
     </row>
     <row r="12" spans="1:20">
-      <c r="A12" s="133" t="s">
+      <c r="A12" s="114" t="s">
         <v>217</v>
       </c>
-      <c r="B12" s="133"/>
-      <c r="C12" s="133">
-        <v>1</v>
-      </c>
-      <c r="D12" s="133"/>
-      <c r="E12" s="133"/>
-      <c r="F12" s="133"/>
-      <c r="G12" s="133"/>
-      <c r="H12" s="133">
-        <v>1</v>
-      </c>
-      <c r="I12" s="133"/>
-      <c r="J12" s="133"/>
-      <c r="K12" s="133"/>
-      <c r="L12" s="133"/>
-      <c r="M12" s="133"/>
-      <c r="P12" s="133">
+      <c r="B12" s="114"/>
+      <c r="C12" s="114">
+        <v>1</v>
+      </c>
+      <c r="D12" s="114"/>
+      <c r="E12" s="114"/>
+      <c r="F12" s="114"/>
+      <c r="G12" s="114"/>
+      <c r="H12" s="114">
+        <v>1</v>
+      </c>
+      <c r="I12" s="114"/>
+      <c r="J12" s="114"/>
+      <c r="K12" s="114"/>
+      <c r="L12" s="114"/>
+      <c r="M12" s="114"/>
+      <c r="P12" s="114">
         <v>2</v>
       </c>
-      <c r="Q12" s="133"/>
-      <c r="R12" s="133"/>
-      <c r="S12" s="133"/>
-      <c r="T12" s="133"/>
+      <c r="Q12" s="114"/>
+      <c r="R12" s="114"/>
+      <c r="S12" s="114"/>
+      <c r="T12" s="114"/>
     </row>
     <row r="13" spans="1:20">
-      <c r="A13" s="133" t="s">
+      <c r="A13" s="114" t="s">
         <v>328</v>
       </c>
-      <c r="B13" s="133"/>
-      <c r="C13" s="133"/>
-      <c r="D13" s="133">
-        <v>1</v>
-      </c>
-      <c r="E13" s="133"/>
-      <c r="F13" s="133">
-        <v>1</v>
-      </c>
-      <c r="G13" s="133"/>
-      <c r="H13" s="133"/>
-      <c r="I13" s="133">
+      <c r="B13" s="114"/>
+      <c r="C13" s="114"/>
+      <c r="D13" s="114">
+        <v>1</v>
+      </c>
+      <c r="E13" s="114"/>
+      <c r="F13" s="114">
+        <v>1</v>
+      </c>
+      <c r="G13" s="114"/>
+      <c r="H13" s="114"/>
+      <c r="I13" s="114">
         <v>5</v>
       </c>
-      <c r="J13" s="133"/>
-      <c r="K13" s="133"/>
-      <c r="L13" s="133"/>
-      <c r="M13" s="133"/>
-      <c r="N13" s="133">
-        <v>1</v>
-      </c>
-      <c r="P13" s="133">
+      <c r="J13" s="114"/>
+      <c r="K13" s="114"/>
+      <c r="L13" s="114"/>
+      <c r="M13" s="114"/>
+      <c r="N13" s="114">
+        <v>1</v>
+      </c>
+      <c r="P13" s="114">
         <v>6</v>
       </c>
-      <c r="Q13" s="133">
-        <v>1</v>
-      </c>
-      <c r="R13" s="133"/>
-      <c r="S13" s="133"/>
-      <c r="T13" s="133"/>
+      <c r="Q13" s="114">
+        <v>1</v>
+      </c>
+      <c r="R13" s="114"/>
+      <c r="S13" s="114"/>
+      <c r="T13" s="114"/>
     </row>
     <row r="14" spans="1:20">
-      <c r="A14" s="133" t="s">
+      <c r="A14" s="114" t="s">
         <v>329</v>
       </c>
-      <c r="B14" s="133"/>
-      <c r="C14" s="133"/>
-      <c r="D14" s="133">
-        <v>1</v>
-      </c>
-      <c r="E14" s="133"/>
-      <c r="F14" s="133">
-        <v>1</v>
-      </c>
-      <c r="G14" s="133"/>
-      <c r="H14" s="133"/>
-      <c r="I14" s="133">
+      <c r="B14" s="114"/>
+      <c r="C14" s="114"/>
+      <c r="D14" s="114">
+        <v>1</v>
+      </c>
+      <c r="E14" s="114"/>
+      <c r="F14" s="114">
+        <v>1</v>
+      </c>
+      <c r="G14" s="114"/>
+      <c r="H14" s="114"/>
+      <c r="I14" s="114">
         <v>5</v>
       </c>
-      <c r="J14" s="133"/>
-      <c r="K14" s="133"/>
-      <c r="L14" s="133"/>
-      <c r="M14" s="133"/>
-      <c r="N14" s="133">
-        <v>1</v>
-      </c>
-      <c r="P14" s="133">
+      <c r="J14" s="114"/>
+      <c r="K14" s="114"/>
+      <c r="L14" s="114"/>
+      <c r="M14" s="114"/>
+      <c r="N14" s="114">
+        <v>1</v>
+      </c>
+      <c r="P14" s="114">
         <v>6</v>
       </c>
-      <c r="Q14" s="133">
-        <v>1</v>
-      </c>
-      <c r="R14" s="133"/>
-      <c r="S14" s="133"/>
-      <c r="T14" s="133"/>
+      <c r="Q14" s="114">
+        <v>1</v>
+      </c>
+      <c r="R14" s="114"/>
+      <c r="S14" s="114"/>
+      <c r="T14" s="114"/>
     </row>
     <row r="15" spans="1:20">
-      <c r="A15" s="133" t="s">
+      <c r="A15" s="114" t="s">
         <v>330</v>
       </c>
-      <c r="B15" s="133"/>
-      <c r="C15" s="133">
-        <v>1</v>
-      </c>
-      <c r="D15" s="133">
-        <v>1</v>
-      </c>
-      <c r="E15" s="133">
-        <v>1</v>
-      </c>
-      <c r="F15" s="133">
+      <c r="B15" s="114"/>
+      <c r="C15" s="114">
+        <v>1</v>
+      </c>
+      <c r="D15" s="114">
+        <v>1</v>
+      </c>
+      <c r="E15" s="114">
+        <v>1</v>
+      </c>
+      <c r="F15" s="114">
         <v>2</v>
       </c>
-      <c r="G15" s="133"/>
-      <c r="H15" s="133"/>
-      <c r="I15" s="133">
+      <c r="G15" s="114"/>
+      <c r="H15" s="114"/>
+      <c r="I15" s="114">
         <v>3</v>
       </c>
-      <c r="J15" s="133"/>
-      <c r="K15" s="133"/>
-      <c r="L15" s="133"/>
-      <c r="M15" s="133"/>
-      <c r="P15" s="133">
+      <c r="J15" s="114"/>
+      <c r="K15" s="114"/>
+      <c r="L15" s="114"/>
+      <c r="M15" s="114"/>
+      <c r="P15" s="114">
         <v>6</v>
       </c>
-      <c r="Q15" s="133">
-        <v>1</v>
-      </c>
-      <c r="R15" s="133"/>
-      <c r="S15" s="133"/>
-      <c r="T15" s="133"/>
+      <c r="Q15" s="114">
+        <v>1</v>
+      </c>
+      <c r="R15" s="114"/>
+      <c r="S15" s="114"/>
+      <c r="T15" s="114"/>
     </row>
     <row r="16" spans="1:20">
-      <c r="A16" s="133" t="s">
+      <c r="A16" s="114" t="s">
         <v>325</v>
       </c>
-      <c r="B16" s="133"/>
-      <c r="C16" s="133"/>
-      <c r="D16" s="133"/>
-      <c r="E16" s="133"/>
-      <c r="F16" s="133"/>
-      <c r="G16" s="133"/>
-      <c r="H16" s="133"/>
-      <c r="I16" s="133"/>
-      <c r="J16" s="133"/>
-      <c r="K16" s="133">
-        <v>1</v>
-      </c>
-      <c r="L16" s="133"/>
-      <c r="M16" s="133"/>
-      <c r="P16" s="133"/>
-      <c r="Q16" s="133"/>
-      <c r="R16" s="133"/>
-      <c r="S16" s="133"/>
-      <c r="T16" s="133"/>
+      <c r="B16" s="114"/>
+      <c r="C16" s="114"/>
+      <c r="D16" s="114"/>
+      <c r="E16" s="114"/>
+      <c r="F16" s="114"/>
+      <c r="G16" s="114"/>
+      <c r="H16" s="114"/>
+      <c r="I16" s="114"/>
+      <c r="J16" s="114"/>
+      <c r="K16" s="114">
+        <v>1</v>
+      </c>
+      <c r="L16" s="114"/>
+      <c r="M16" s="114"/>
+      <c r="P16" s="114"/>
+      <c r="Q16" s="114"/>
+      <c r="R16" s="114"/>
+      <c r="S16" s="114"/>
+      <c r="T16" s="114"/>
     </row>
     <row r="17" spans="1:20">
-      <c r="A17" s="133"/>
-      <c r="B17" s="133"/>
-      <c r="C17" s="133"/>
-      <c r="D17" s="133"/>
-      <c r="E17" s="133"/>
-      <c r="F17" s="133"/>
-      <c r="G17" s="133"/>
-      <c r="H17" s="133"/>
-      <c r="I17" s="133"/>
-      <c r="J17" s="133"/>
-      <c r="K17" s="133"/>
-      <c r="L17" s="133"/>
-      <c r="M17" s="133"/>
-      <c r="P17" s="133"/>
-      <c r="Q17" s="133"/>
-      <c r="R17" s="133"/>
-      <c r="S17" s="133"/>
-      <c r="T17" s="133"/>
+      <c r="A17" s="114"/>
+      <c r="B17" s="114"/>
+      <c r="C17" s="114"/>
+      <c r="D17" s="114"/>
+      <c r="E17" s="114"/>
+      <c r="F17" s="114"/>
+      <c r="G17" s="114"/>
+      <c r="H17" s="114"/>
+      <c r="I17" s="114"/>
+      <c r="J17" s="114"/>
+      <c r="K17" s="114"/>
+      <c r="L17" s="114"/>
+      <c r="M17" s="114"/>
+      <c r="P17" s="114"/>
+      <c r="Q17" s="114"/>
+      <c r="R17" s="114"/>
+      <c r="S17" s="114"/>
+      <c r="T17" s="114"/>
     </row>
     <row r="18" spans="1:20">
-      <c r="A18" s="133"/>
-      <c r="B18" s="133"/>
-      <c r="C18" s="133"/>
-      <c r="D18" s="133"/>
-      <c r="E18" s="133"/>
-      <c r="F18" s="133"/>
-      <c r="G18" s="133"/>
-      <c r="H18" s="133"/>
-      <c r="I18" s="133"/>
-      <c r="J18" s="133"/>
-      <c r="K18" s="133"/>
-      <c r="L18" s="133"/>
-      <c r="M18" s="133"/>
-      <c r="P18" s="133"/>
-      <c r="Q18" s="133"/>
-      <c r="R18" s="133"/>
-      <c r="S18" s="133"/>
-      <c r="T18" s="133"/>
+      <c r="A18" s="134"/>
+      <c r="B18" s="134"/>
+      <c r="C18" s="134">
+        <f>SUM([Włącznik 1])</f>
+        <v>13</v>
+      </c>
+      <c r="D18" s="134">
+        <f>SUM([Włącznik 2])</f>
+        <v>6</v>
+      </c>
+      <c r="E18" s="134">
+        <f>SUM([W krzyżowy])</f>
+        <v>3</v>
+      </c>
+      <c r="F18" s="134">
+        <f>SUM([W schodowy 1])</f>
+        <v>10</v>
+      </c>
+      <c r="G18" s="134">
+        <f>SUM([W schodowy 2])</f>
+        <v>2</v>
+      </c>
+      <c r="H18" s="134">
+        <f>SUM([Gniazdko 1])</f>
+        <v>8</v>
+      </c>
+      <c r="I18" s="134">
+        <f>SUM([Gniazdko 2])</f>
+        <v>26</v>
+      </c>
+      <c r="J18" s="134">
+        <f>SUM([Gniazdko H])</f>
+        <v>10</v>
+      </c>
+      <c r="K18" s="134">
+        <f>SUM([Natynkowe])</f>
+        <v>1</v>
+      </c>
+      <c r="L18" s="134">
+        <f>SUM([Głośnik 1])</f>
+        <v>4</v>
+      </c>
+      <c r="M18" s="134">
+        <f>SUM([Głośnik 2])</f>
+        <v>2</v>
+      </c>
+      <c r="N18" s="134">
+        <f>SUM([Sat])</f>
+        <v>4</v>
+      </c>
+      <c r="O18" s="134">
+        <f>SUM([komp])</f>
+        <v>1</v>
+      </c>
+      <c r="P18" s="134">
+        <f>SUM([Ramka1])</f>
+        <v>37</v>
+      </c>
+      <c r="Q18" s="134">
+        <f>SUM([Ramka2])</f>
+        <v>16</v>
+      </c>
+      <c r="R18" s="134">
+        <f>SUM([Ramka3])</f>
+        <v>4</v>
+      </c>
+      <c r="S18" s="134">
+        <f>SUM([Ramka4])</f>
+        <v>0</v>
+      </c>
+      <c r="T18" s="134">
+        <f>SUM([Ramka5])</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="20" spans="1:20">
       <c r="A20" t="s">
@@ -5630,10 +6005,10 @@
       <c r="M20" t="s">
         <v>217</v>
       </c>
-      <c r="N20" s="133" t="s">
+      <c r="N20" s="114" t="s">
         <v>328</v>
       </c>
-      <c r="O20" s="133" t="s">
+      <c r="O20" s="114" t="s">
         <v>329</v>
       </c>
       <c r="P20" t="s">
@@ -5693,10 +6068,10 @@
       <c r="G22">
         <v>1</v>
       </c>
-      <c r="N22" s="133">
-        <v>1</v>
-      </c>
-      <c r="O22" s="133">
+      <c r="N22" s="114">
+        <v>1</v>
+      </c>
+      <c r="O22" s="114">
         <v>1</v>
       </c>
       <c r="P22">
@@ -5738,10 +6113,10 @@
       <c r="L24">
         <v>2</v>
       </c>
-      <c r="N24" s="133">
-        <v>1</v>
-      </c>
-      <c r="O24" s="133">
+      <c r="N24" s="114">
+        <v>1</v>
+      </c>
+      <c r="O24" s="114">
         <v>1</v>
       </c>
       <c r="P24">
@@ -5810,10 +6185,10 @@
       <c r="L27">
         <v>1</v>
       </c>
-      <c r="N27" s="133">
+      <c r="N27" s="114">
         <v>5</v>
       </c>
-      <c r="O27" s="133">
+      <c r="O27" s="114">
         <v>5</v>
       </c>
       <c r="P27">
@@ -5882,10 +6257,10 @@
       <c r="F32">
         <v>2</v>
       </c>
-      <c r="N32" s="133">
-        <v>1</v>
-      </c>
-      <c r="O32" s="133">
+      <c r="N32" s="114">
+        <v>1</v>
+      </c>
+      <c r="O32" s="114">
         <v>1</v>
       </c>
     </row>
@@ -5936,10 +6311,10 @@
       <c r="M34">
         <v>2</v>
       </c>
-      <c r="N34" s="133">
+      <c r="N34" s="114">
         <v>6</v>
       </c>
-      <c r="O34" s="133">
+      <c r="O34" s="114">
         <v>6</v>
       </c>
       <c r="P34">
@@ -5975,10 +6350,10 @@
       <c r="L35">
         <v>1</v>
       </c>
-      <c r="N35" s="133">
-        <v>1</v>
-      </c>
-      <c r="O35" s="133">
+      <c r="N35" s="114">
+        <v>1</v>
+      </c>
+      <c r="O35" s="114">
         <v>1</v>
       </c>
       <c r="P35">

</xml_diff>